<commit_message>
WORK-IN-PROGRESS FLOWreports_PEST_LittleNSantiam50.xml - Add "FLOW NSantiam temperature skill assessment monthly" report. Flow.cpp, .h - Remove m_fluxWP as a member of class FluxContainer; replace it with m_additionsWP as a member of class Reach. Add AccumAdditions(WP) and AccumWithdrawals(m3) as methods of Reach. Move the body of Reach::AddFluxFromGlobalHandler() from Flow.h to Flow.cpp. FluxExpr.cpp - Replace m_fluxWP with m_additionsWP. Put logic into FluxExpr::Step() and Spring::Step() to handle water going into the reach without losing its temperature. ReachRouting.cpp, GlobalMethods.h - Add ReachRouting::GetAdditionsToReach(). In SolveReachKinematicWave(), mix in the "lateral" additions to the reach, then take out the lateral withdrawals from the reach, before applying the energy fluxes. Add ReachRouting::GetAdditionsToReach()
</commit_message>
<xml_diff>
--- a/DataCW3M/SkillAssessment/Temp72monthsStatisticsCalculator.xlsx
+++ b/DataCW3M/SkillAssessment/Temp72monthsStatisticsCalculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\SkillAssessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B9A0D03-5826-44EF-8C9E-8A937873B605}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0B530B-DF5C-46AA-9963-4F275BCBB17E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -860,223 +860,223 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="73"/>
                 <c:pt idx="0">
-                  <c:v>6.3707539999999998</c:v>
+                  <c:v>5.6333679999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.486688</c:v>
+                  <c:v>5.8525710000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.5915010000000001</c:v>
+                  <c:v>5.9628100000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.9977999999999998</c:v>
+                  <c:v>6.5337459999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.3669480000000007</c:v>
+                  <c:v>8.5463539999999991</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.893663999999999</c:v>
+                  <c:v>12.305540000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14.632066999999999</c:v>
+                  <c:v>17.797739</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14.734399</c:v>
+                  <c:v>17.887530999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12.294855</c:v>
+                  <c:v>14.438943</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.6366829999999997</c:v>
+                  <c:v>10.489164000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6.154617</c:v>
+                  <c:v>5.3780950000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.0597560000000001</c:v>
+                  <c:v>3.7197469999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.3405769999999997</c:v>
+                  <c:v>4.213533</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.6972199999999997</c:v>
+                  <c:v>3.3110390000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.7556729999999998</c:v>
+                  <c:v>4.7018979999999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.8229920000000002</c:v>
+                  <c:v>4.7580549999999997</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8.1870809999999992</c:v>
+                  <c:v>8.2818780000000007</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>11.771432000000001</c:v>
+                  <c:v>13.595072999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>13.539778999999999</c:v>
+                  <c:v>16.21734</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>14.614145000000001</c:v>
+                  <c:v>17.771920999999999</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>14.221209</c:v>
+                  <c:v>17.381886000000002</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>9.4169959999999993</c:v>
+                  <c:v>10.232779000000001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>5.7774590000000003</c:v>
+                  <c:v>4.8344560000000003</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>5.1599469999999998</c:v>
+                  <c:v>4.0301580000000001</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>4.8252810000000004</c:v>
+                  <c:v>3.4191470000000002</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>5.2225970000000004</c:v>
+                  <c:v>3.9419179999999998</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4.6455700000000002</c:v>
+                  <c:v>3.101648</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>8.1837680000000006</c:v>
+                  <c:v>8.2963290000000001</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>9.8008500000000005</c:v>
+                  <c:v>10.669551999999999</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>10.984868000000001</c:v>
+                  <c:v>12.462146000000001</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>14.640597</c:v>
+                  <c:v>17.817267999999999</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>15.450846</c:v>
+                  <c:v>18.962933</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>13.818787</c:v>
+                  <c:v>16.609960999999998</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>9.8301639999999999</c:v>
+                  <c:v>10.76773</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>7.1806229999999998</c:v>
+                  <c:v>6.8409709999999997</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>4.2529050000000002</c:v>
+                  <c:v>2.559825</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4.5596059999999996</c:v>
+                  <c:v>3.1383709999999998</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4.6835370000000003</c:v>
+                  <c:v>3.2248890000000001</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>6.7431599999999996</c:v>
+                  <c:v>6.1851079999999996</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>7.9069370000000001</c:v>
+                  <c:v>7.8967999999999998</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>10.611583</c:v>
+                  <c:v>11.922974</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>12.615589</c:v>
+                  <c:v>14.898326000000001</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>15.329357</c:v>
+                  <c:v>18.877089000000002</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>15.468318</c:v>
+                  <c:v>19.143405999999999</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>12.845349000000001</c:v>
+                  <c:v>15.331623</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>9.2232450000000004</c:v>
+                  <c:v>9.8799829999999993</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>6.4217240000000002</c:v>
+                  <c:v>5.785768</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>4.9075059999999997</c:v>
+                  <c:v>3.7002160000000002</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>6.6897539999999998</c:v>
+                  <c:v>6.1772119999999999</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>5.1091240000000004</c:v>
+                  <c:v>3.8808240000000001</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>6.7198719999999996</c:v>
+                  <c:v>6.1220439999999998</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>8.1393380000000004</c:v>
+                  <c:v>8.2367699999999999</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>10.965527</c:v>
+                  <c:v>12.453976000000001</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>12.090954999999999</c:v>
+                  <c:v>14.089005999999999</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>15.754887</c:v>
+                  <c:v>19.526872999999998</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>15.936168</c:v>
+                  <c:v>19.820018999999998</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>13.682073000000001</c:v>
+                  <c:v>16.607327000000002</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>11.03308</c:v>
+                  <c:v>12.605307</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>6.8393689999999996</c:v>
+                  <c:v>6.3983939999999997</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>6.1479119999999998</c:v>
+                  <c:v>5.3554399999999998</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>7.7735810000000001</c:v>
+                  <c:v>7.7686400000000004</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>7.9811069999999997</c:v>
+                  <c:v>8.0858450000000008</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>8.9005240000000008</c:v>
+                  <c:v>9.4184230000000007</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>8.0581899999999997</c:v>
+                  <c:v>8.124053</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>11.277295000000001</c:v>
+                  <c:v>12.881795</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>15.160458</c:v>
+                  <c:v>18.613572999999999</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>16.247042</c:v>
+                  <c:v>20.134067999999999</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>15.759136</c:v>
+                  <c:v>19.531728999999999</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>12.396628</c:v>
+                  <c:v>14.65448</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>11.708904</c:v>
+                  <c:v>13.600369000000001</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>5.8872299999999997</c:v>
+                  <c:v>4.9770370000000002</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>5.1732170000000002</c:v>
+                  <c:v>3.8891260000000001</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>5.0393340000000002</c:v>
+                  <c:v>3.7530060000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3539,7 +3539,7 @@
   <dimension ref="A1:AD3254"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D75"/>
+      <selection activeCell="H3" sqref="H3:I111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3575,7 +3575,7 @@
       </c>
       <c r="B2" s="9">
         <f>H2-I2</f>
-        <v>-1.3066063194444411</v>
+        <v>-0.55447361111110638</v>
       </c>
       <c r="D2" t="s">
         <v>17</v>
@@ -3585,7 +3585,7 @@
       <c r="G2"/>
       <c r="H2">
         <f>AVERAGE(H4:H75)</f>
-        <v>9.4181719444444454</v>
+        <v>10.17030465277778</v>
       </c>
       <c r="I2">
         <f>AVERAGE(I4:I75)</f>
@@ -3599,12 +3599,12 @@
       <c r="O2" s="4"/>
       <c r="P2" s="4">
         <f>AVERAGE(P4:P75)</f>
-        <v>5.6629607613288737</v>
+        <v>1.9901857859469727</v>
       </c>
       <c r="Q2" s="4"/>
       <c r="R2" s="4">
         <f>AVERAGE(R4:R75)</f>
-        <v>1.6840875138888889</v>
+        <v>1.1719316666666668</v>
       </c>
       <c r="S2">
         <f>AVERAGE(S4:S75)</f>
@@ -3623,11 +3623,11 @@
       </c>
       <c r="B3" s="11">
         <f>(I2-H2)/H2</f>
-        <v>0.13873247665808192</v>
+        <v>5.4518879231377292E-2</v>
       </c>
       <c r="C3" s="8" t="str">
         <f>IF(ABS(B3)&lt;5%,"VG",IF(ABS(B3)&lt;10%,"G",IF(ABS(B3)&lt;15%,"S","NS")))</f>
-        <v>S</v>
+        <v>G</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>0</v>
@@ -3711,7 +3711,7 @@
       </c>
       <c r="B4" s="1">
         <f>1-SUM(P4:P75)/SUM(M4:M75)</f>
-        <v>0.80598273675024246</v>
+        <v>0.93181474924128027</v>
       </c>
       <c r="C4" s="7" t="str">
         <f>IF(B4&gt;0.8,"VG",IF(B4&gt;0.7,"G",IF(B4&gt;0.45,"S","NS")))</f>
@@ -3730,14 +3730,14 @@
         <v>31</v>
       </c>
       <c r="H4">
-        <v>6.3707539999999998</v>
+        <v>5.6333679999999999</v>
       </c>
       <c r="I4">
         <v>6.5488150000000003</v>
       </c>
       <c r="J4" s="2">
         <f>I4-H4</f>
-        <v>0.17806100000000047</v>
+        <v>0.91544700000000034</v>
       </c>
       <c r="K4" s="2">
         <f>I4-I$2</f>
@@ -3745,7 +3745,7 @@
       </c>
       <c r="L4" s="2">
         <f>H4-H$2</f>
-        <v>-3.0474179444444456</v>
+        <v>-4.5369366527777801</v>
       </c>
       <c r="M4" s="2">
         <f>K4*K4</f>
@@ -3753,23 +3753,23 @@
       </c>
       <c r="N4" s="2">
         <f>L4*L4</f>
-        <v>9.2867561281220095</v>
+        <v>20.583794191318447</v>
       </c>
       <c r="O4" s="2">
         <f>K4*L4</f>
-        <v>12.725905385715787</v>
+        <v>18.946080792591015</v>
       </c>
       <c r="P4" s="2">
         <f>J4*J4</f>
-        <v>3.170571972100017E-2</v>
+        <v>0.8380432098090006</v>
       </c>
       <c r="Q4" s="2">
         <f>(I4-H$2)*(I4-H$2)</f>
-        <v>8.2332092746315624</v>
+        <v>13.115187305176525</v>
       </c>
       <c r="R4" s="2">
         <f>ABS(J4)</f>
-        <v>0.17806100000000047</v>
+        <v>0.91544700000000034</v>
       </c>
       <c r="S4">
         <v>5.1376660000000003</v>
@@ -3810,7 +3810,7 @@
       </c>
       <c r="B5" s="1">
         <f>SQRT(SUM(P4:P75))/SQRT(SUM(Q4:Q75))</f>
-        <v>0.42813100202930987</v>
+        <v>0.25975860117791605</v>
       </c>
       <c r="C5" s="7" t="str">
         <f>IF(B5&lt;=0.5,"VG",IF(B5&lt;=0.6,"G",IF(B5&lt;=0.7,"S","NS")))</f>
@@ -3829,14 +3829,14 @@
         <v>28</v>
       </c>
       <c r="H5">
-        <v>6.486688</v>
+        <v>5.8525710000000002</v>
       </c>
       <c r="I5">
         <v>6.2569530000000002</v>
       </c>
       <c r="J5" s="2">
         <f t="shared" ref="J5:J39" si="0">I5-H5</f>
-        <v>-0.2297349999999998</v>
+        <v>0.40438200000000002</v>
       </c>
       <c r="K5" s="2">
         <f t="shared" ref="K5:K39" si="1">I5-I$2</f>
@@ -3844,7 +3844,7 @@
       </c>
       <c r="L5" s="2">
         <f t="shared" ref="L5:L39" si="2">H5-H$2</f>
-        <v>-2.9314839444444454</v>
+        <v>-4.3177336527777799</v>
       </c>
       <c r="M5" s="2">
         <f t="shared" ref="M5:M39" si="3">K5*K5</f>
@@ -3852,23 +3852,23 @@
       </c>
       <c r="N5" s="2">
         <f t="shared" ref="N5:N39" si="4">L5*L5</f>
-        <v>8.5935981165355635</v>
+        <v>18.642823896329748</v>
       </c>
       <c r="O5" s="2">
         <f t="shared" ref="O5:O39" si="5">K5*L5</f>
-        <v>13.097358027673538</v>
+        <v>19.290879496623809</v>
       </c>
       <c r="P5" s="2">
         <f t="shared" ref="P5:P39" si="6">J5*J5</f>
-        <v>5.2778170224999907E-2</v>
+        <v>0.16352480192400001</v>
       </c>
       <c r="Q5" s="2">
         <f t="shared" ref="Q5:Q39" si="7">(I5-H$2)*(I5-H$2)</f>
-        <v>9.9933052147144519</v>
+        <v>15.314321158298581</v>
       </c>
       <c r="R5" s="2">
         <f t="shared" ref="R5:R39" si="8">ABS(J5)</f>
-        <v>0.2297349999999998</v>
+        <v>0.40438200000000002</v>
       </c>
       <c r="S5">
         <v>5.2818040000000002</v>
@@ -3909,7 +3909,7 @@
       </c>
       <c r="B6" s="10">
         <f>B12*B12</f>
-        <v>0.94397896272708892</v>
+        <v>0.94424347034452072</v>
       </c>
       <c r="C6" s="7" t="str">
         <f>IF(B6&gt;0.85,"VG",IF(B6&gt;0.75,"G",IF(B6&gt;0.6,"S","NS")))</f>
@@ -3928,14 +3928,14 @@
         <v>31</v>
       </c>
       <c r="H6">
-        <v>6.5915010000000001</v>
+        <v>5.9628100000000002</v>
       </c>
       <c r="I6">
         <v>6.5102969999999996</v>
       </c>
       <c r="J6" s="2">
         <f t="shared" si="0"/>
-        <v>-8.1204000000000498E-2</v>
+        <v>0.54748699999999939</v>
       </c>
       <c r="K6" s="2">
         <f t="shared" si="1"/>
@@ -3943,7 +3943,7 @@
       </c>
       <c r="L6" s="2">
         <f t="shared" si="2"/>
-        <v>-2.8266709444444453</v>
+        <v>-4.2074946527777799</v>
       </c>
       <c r="M6" s="2">
         <f t="shared" si="3"/>
@@ -3951,23 +3951,23 @@
       </c>
       <c r="N6" s="2">
         <f t="shared" si="4"/>
-        <v>7.9900686281664521</v>
+        <v>17.703011253153612</v>
       </c>
       <c r="O6" s="2">
         <f t="shared" si="5"/>
-        <v>11.91295173454022</v>
+        <v>17.732407382044631</v>
       </c>
       <c r="P6" s="2">
         <f t="shared" si="6"/>
-        <v>6.5940896160000808E-3</v>
+        <v>0.29974201516899934</v>
       </c>
       <c r="Q6" s="2">
         <f t="shared" si="7"/>
-        <v>8.4557366925277897</v>
+        <v>13.395656018391918</v>
       </c>
       <c r="R6" s="2">
         <f t="shared" si="8"/>
-        <v>8.1204000000000498E-2</v>
+        <v>0.54748699999999939</v>
       </c>
       <c r="S6">
         <v>5.855613</v>
@@ -4008,7 +4008,7 @@
       </c>
       <c r="B7" s="1">
         <f>H2</f>
-        <v>9.4181719444444454</v>
+        <v>10.17030465277778</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7">
@@ -4024,14 +4024,14 @@
         <v>30</v>
       </c>
       <c r="H7">
-        <v>6.9977999999999998</v>
+        <v>6.5337459999999998</v>
       </c>
       <c r="I7">
         <v>7.016629</v>
       </c>
       <c r="J7" s="2">
         <f t="shared" si="0"/>
-        <v>1.8829000000000207E-2</v>
+        <v>0.48288300000000017</v>
       </c>
       <c r="K7" s="2">
         <f t="shared" si="1"/>
@@ -4039,7 +4039,7 @@
       </c>
       <c r="L7" s="2">
         <f t="shared" si="2"/>
-        <v>-2.4203719444444456</v>
+        <v>-3.6365586527777802</v>
       </c>
       <c r="M7" s="2">
         <f t="shared" si="3"/>
@@ -4047,23 +4047,23 @@
       </c>
       <c r="N7" s="2">
         <f t="shared" si="4"/>
-        <v>5.858200349453786</v>
+        <v>13.224558835092944</v>
       </c>
       <c r="O7" s="2">
         <f t="shared" si="5"/>
-        <v>8.9751004441289837</v>
+        <v>13.484902291386687</v>
       </c>
       <c r="P7" s="2">
         <f t="shared" si="6"/>
-        <v>3.5453124100000776E-4</v>
+        <v>0.23317599168900016</v>
       </c>
       <c r="Q7" s="2">
         <f t="shared" si="7"/>
-        <v>5.7674085140108966</v>
+        <v>9.9456701229233566</v>
       </c>
       <c r="R7" s="2">
         <f t="shared" si="8"/>
-        <v>1.8829000000000207E-2</v>
+        <v>0.48288300000000017</v>
       </c>
       <c r="S7">
         <v>6.2127059999999998</v>
@@ -4104,7 +4104,7 @@
       </c>
       <c r="B8" s="1">
         <f>_xlfn.STDEV.P(H4:H75)</f>
-        <v>3.7257220655702734</v>
+        <v>5.4850280873380894</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8">
@@ -4120,14 +4120,14 @@
         <v>31</v>
       </c>
       <c r="H8">
-        <v>8.3669480000000007</v>
+        <v>8.5463539999999991</v>
       </c>
       <c r="I8">
         <v>8.5420350000000003</v>
       </c>
       <c r="J8" s="2">
         <f t="shared" si="0"/>
-        <v>0.17508699999999955</v>
+        <v>-4.3189999999988515E-3</v>
       </c>
       <c r="K8" s="2">
         <f t="shared" si="1"/>
@@ -4135,7 +4135,7 @@
       </c>
       <c r="L8" s="2">
         <f t="shared" si="2"/>
-        <v>-1.0512239444444447</v>
+        <v>-1.6239506527777809</v>
       </c>
       <c r="M8" s="2">
         <f t="shared" si="3"/>
@@ -4143,23 +4143,23 @@
       </c>
       <c r="N8" s="2">
         <f t="shared" si="4"/>
-        <v>1.1050717813733368</v>
+        <v>2.6372157226573809</v>
       </c>
       <c r="O8" s="2">
         <f t="shared" si="5"/>
-        <v>2.2945519835748165</v>
+        <v>3.544667348238661</v>
       </c>
       <c r="P8" s="2">
         <f t="shared" si="6"/>
-        <v>3.0655457568999841E-2</v>
+        <v>1.865376099999008E-5</v>
       </c>
       <c r="Q8" s="2">
         <f t="shared" si="7"/>
-        <v>0.76761594542044875</v>
+        <v>2.6512620621570715</v>
       </c>
       <c r="R8" s="2">
         <f t="shared" si="8"/>
-        <v>0.17508699999999955</v>
+        <v>4.3189999999988515E-3</v>
       </c>
       <c r="S8">
         <v>6.9663380000000004</v>
@@ -4216,14 +4216,14 @@
         <v>30</v>
       </c>
       <c r="H9">
-        <v>10.893663999999999</v>
+        <v>12.305540000000001</v>
       </c>
       <c r="I9">
         <v>11.353870000000001</v>
       </c>
       <c r="J9" s="2">
         <f t="shared" si="0"/>
-        <v>0.46020600000000123</v>
+        <v>-0.95167000000000002</v>
       </c>
       <c r="K9" s="2">
         <f t="shared" si="1"/>
@@ -4231,7 +4231,7 @@
       </c>
       <c r="L9" s="2">
         <f t="shared" si="2"/>
-        <v>1.475492055555554</v>
+        <v>2.1352353472222205</v>
       </c>
       <c r="M9" s="2">
         <f t="shared" si="3"/>
@@ -4239,23 +4239,23 @@
       </c>
       <c r="N9" s="2">
         <f t="shared" si="4"/>
-        <v>2.177076806007554</v>
+        <v>4.5592299880271963</v>
       </c>
       <c r="O9" s="2">
         <f t="shared" si="5"/>
-        <v>0.92821985884759994</v>
+        <v>1.3432589115898443</v>
       </c>
       <c r="P9" s="2">
         <f t="shared" si="6"/>
-        <v>0.21178956243600114</v>
+        <v>0.9056757889</v>
       </c>
       <c r="Q9" s="2">
         <f t="shared" si="7"/>
-        <v>3.7469269622815573</v>
+        <v>1.4008269311452555</v>
       </c>
       <c r="R9" s="2">
         <f t="shared" si="8"/>
-        <v>0.46020600000000123</v>
+        <v>0.95167000000000002</v>
       </c>
       <c r="S9">
         <v>8.0567130000000002</v>
@@ -4311,14 +4311,14 @@
         <v>31</v>
       </c>
       <c r="H10">
-        <v>14.632066999999999</v>
+        <v>17.797739</v>
       </c>
       <c r="I10">
         <v>18.857621999999999</v>
       </c>
       <c r="J10" s="2">
         <f t="shared" si="0"/>
-        <v>4.2255549999999999</v>
+        <v>1.0598829999999992</v>
       </c>
       <c r="K10" s="2">
         <f t="shared" si="1"/>
@@ -4326,7 +4326,7 @@
       </c>
       <c r="L10" s="2">
         <f t="shared" si="2"/>
-        <v>5.2138950555555539</v>
+        <v>7.6274343472222199</v>
       </c>
       <c r="M10" s="2">
         <f t="shared" si="3"/>
@@ -4334,23 +4334,23 @@
       </c>
       <c r="N10" s="2">
         <f t="shared" si="4"/>
-        <v>27.184701650346653</v>
+        <v>58.177754721185252</v>
       </c>
       <c r="O10" s="2">
         <f t="shared" si="5"/>
-        <v>42.403793743315688</v>
+        <v>62.032731653404987</v>
       </c>
       <c r="P10" s="2">
         <f t="shared" si="6"/>
-        <v>17.855315058024999</v>
+        <v>1.1233519736889983</v>
       </c>
       <c r="Q10" s="2">
         <f t="shared" si="7"/>
-        <v>89.103217351327743</v>
+        <v>75.469482691348091</v>
       </c>
       <c r="R10" s="2">
         <f t="shared" si="8"/>
-        <v>4.2255549999999999</v>
+        <v>1.0598829999999992</v>
       </c>
       <c r="S10">
         <v>10.862743</v>
@@ -4391,7 +4391,7 @@
       </c>
       <c r="B11" s="1">
         <f>SQRT(P$2)</f>
-        <v>2.3796976197258495</v>
+        <v>1.4107394465127048</v>
       </c>
       <c r="D11">
         <v>7</v>
@@ -4406,14 +4406,14 @@
         <v>31</v>
       </c>
       <c r="H11">
-        <v>14.734399</v>
+        <v>17.887530999999999</v>
       </c>
       <c r="I11">
         <v>19.686464000000001</v>
       </c>
       <c r="J11" s="2">
         <f t="shared" si="0"/>
-        <v>4.952065000000001</v>
+        <v>1.7989330000000017</v>
       </c>
       <c r="K11" s="2">
         <f t="shared" si="1"/>
@@ -4421,7 +4421,7 @@
       </c>
       <c r="L11" s="2">
         <f t="shared" si="2"/>
-        <v>5.3162270555555544</v>
+        <v>7.7172263472222191</v>
       </c>
       <c r="M11" s="2">
         <f t="shared" si="3"/>
@@ -4429,23 +4429,23 @@
       </c>
       <c r="N11" s="2">
         <f t="shared" si="4"/>
-        <v>28.262270106220878</v>
+        <v>59.555582494260797</v>
       </c>
       <c r="O11" s="2">
         <f t="shared" si="5"/>
-        <v>47.6423561737002</v>
+        <v>69.15935727824224</v>
       </c>
       <c r="P11" s="2">
         <f t="shared" si="6"/>
-        <v>24.522947764225009</v>
+        <v>3.2361599384890058</v>
       </c>
       <c r="Q11" s="2">
         <f t="shared" si="7"/>
-        <v>105.43782173818533</v>
+        <v>90.557288721724845</v>
       </c>
       <c r="R11" s="2">
         <f t="shared" si="8"/>
-        <v>4.952065000000001</v>
+        <v>1.7989330000000017</v>
       </c>
       <c r="S11">
         <v>13.279059</v>
@@ -4486,7 +4486,7 @@
       </c>
       <c r="B12" s="1">
         <f>SUM(O4:O75)/SQRT(SUM(M4:M75)*SUM(N4:N75))</f>
-        <v>0.9715857979237289</v>
+        <v>0.97172190998480668</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12">
@@ -4502,14 +4502,14 @@
         <v>30</v>
       </c>
       <c r="H12">
-        <v>12.294855</v>
+        <v>14.438943</v>
       </c>
       <c r="I12">
         <v>15.759565</v>
       </c>
       <c r="J12" s="2">
         <f t="shared" si="0"/>
-        <v>3.4647100000000002</v>
+        <v>1.3206220000000002</v>
       </c>
       <c r="K12" s="2">
         <f t="shared" si="1"/>
@@ -4517,7 +4517,7 @@
       </c>
       <c r="L12" s="2">
         <f t="shared" si="2"/>
-        <v>2.8766830555555547</v>
+        <v>4.26863834722222</v>
       </c>
       <c r="M12" s="2">
         <f t="shared" si="3"/>
@@ -4525,23 +4525,23 @@
       </c>
       <c r="N12" s="2">
         <f t="shared" si="4"/>
-        <v>8.2753054021204431</v>
+        <v>18.221273339376047</v>
       </c>
       <c r="O12" s="2">
         <f t="shared" si="5"/>
-        <v>14.483485692106697</v>
+        <v>21.491683731849701</v>
       </c>
       <c r="P12" s="2">
         <f t="shared" si="6"/>
-        <v>12.004215384100002</v>
+        <v>1.7440424668840004</v>
       </c>
       <c r="Q12" s="2">
         <f t="shared" si="7"/>
-        <v>40.213265885048216</v>
+        <v>31.239831229030653</v>
       </c>
       <c r="R12" s="2">
         <f t="shared" si="8"/>
-        <v>3.4647100000000002</v>
+        <v>1.3206220000000002</v>
       </c>
       <c r="S12">
         <v>13.139711999999999</v>
@@ -4582,7 +4582,7 @@
       </c>
       <c r="B13" s="2">
         <f>R2</f>
-        <v>1.6840875138888889</v>
+        <v>1.1719316666666668</v>
       </c>
       <c r="D13">
         <v>9</v>
@@ -4597,14 +4597,14 @@
         <v>31</v>
       </c>
       <c r="H13">
-        <v>9.6366829999999997</v>
+        <v>10.489164000000001</v>
       </c>
       <c r="I13">
         <v>11.111582</v>
       </c>
       <c r="J13" s="2">
         <f t="shared" si="0"/>
-        <v>1.4748990000000006</v>
+        <v>0.62241799999999969</v>
       </c>
       <c r="K13" s="2">
         <f t="shared" si="1"/>
@@ -4612,7 +4612,7 @@
       </c>
       <c r="L13" s="2">
         <f t="shared" si="2"/>
-        <v>0.21851105555555428</v>
+        <v>0.31885934722222053</v>
       </c>
       <c r="M13" s="2">
         <f t="shared" si="3"/>
@@ -4620,23 +4620,23 @@
       </c>
       <c r="N13" s="2">
         <f t="shared" si="4"/>
-        <v>4.7747081400002528E-2</v>
+        <v>0.1016712833109806</v>
       </c>
       <c r="O13" s="2">
         <f t="shared" si="5"/>
-        <v>8.4520892670471554E-2</v>
+        <v>0.12333598679950582</v>
       </c>
       <c r="P13" s="2">
         <f t="shared" si="6"/>
-        <v>2.1753270602010017</v>
+        <v>0.38740416672399963</v>
       </c>
       <c r="Q13" s="2">
         <f t="shared" si="7"/>
-        <v>2.8676376162566677</v>
+        <v>0.88600304439370015</v>
       </c>
       <c r="R13" s="2">
         <f t="shared" si="8"/>
-        <v>1.4748990000000006</v>
+        <v>0.62241799999999969</v>
       </c>
       <c r="S13">
         <v>12.061854</v>
@@ -4685,14 +4685,14 @@
         <v>30</v>
       </c>
       <c r="H14">
-        <v>6.154617</v>
+        <v>5.3780950000000001</v>
       </c>
       <c r="I14">
         <v>7.2814439999999996</v>
       </c>
       <c r="J14" s="2">
         <f t="shared" si="0"/>
-        <v>1.1268269999999996</v>
+        <v>1.9033489999999995</v>
       </c>
       <c r="K14" s="2">
         <f t="shared" si="1"/>
@@ -4700,7 +4700,7 @@
       </c>
       <c r="L14" s="2">
         <f t="shared" si="2"/>
-        <v>-3.2635549444444454</v>
+        <v>-4.79220965277778</v>
       </c>
       <c r="M14" s="2">
         <f t="shared" si="3"/>
@@ -4708,23 +4708,23 @@
       </c>
       <c r="N14" s="2">
         <f t="shared" si="4"/>
-        <v>10.650790875407788</v>
+        <v>22.965273356176532</v>
       </c>
       <c r="O14" s="2">
         <f t="shared" si="5"/>
-        <v>11.237510562289552</v>
+        <v>16.501179697148796</v>
       </c>
       <c r="P14" s="2">
         <f t="shared" si="6"/>
-        <v>1.2697390879289991</v>
+        <v>3.622737415800998</v>
       </c>
       <c r="Q14" s="2">
         <f t="shared" si="7"/>
-        <v>4.5656063085697864</v>
+        <v>8.3455158711676631</v>
       </c>
       <c r="R14" s="2">
         <f t="shared" si="8"/>
-        <v>1.1268269999999996</v>
+        <v>1.9033489999999995</v>
       </c>
       <c r="S14">
         <v>5.7312029999999998</v>
@@ -4762,7 +4762,7 @@
     <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B15" s="6">
         <f>B5</f>
-        <v>0.42813100202930987</v>
+        <v>0.25975860117791605</v>
       </c>
       <c r="D15">
         <v>11</v>
@@ -4777,14 +4777,14 @@
         <v>31</v>
       </c>
       <c r="H15">
-        <v>5.0597560000000001</v>
+        <v>3.7197469999999999</v>
       </c>
       <c r="I15">
         <v>6.213406</v>
       </c>
       <c r="J15" s="2">
         <f t="shared" si="0"/>
-        <v>1.1536499999999998</v>
+        <v>2.4936590000000001</v>
       </c>
       <c r="K15" s="2">
         <f t="shared" si="1"/>
@@ -4792,7 +4792,7 @@
       </c>
       <c r="L15" s="2">
         <f t="shared" si="2"/>
-        <v>-4.3584159444444452</v>
+        <v>-6.4505576527777801</v>
       </c>
       <c r="M15" s="2">
         <f t="shared" si="3"/>
@@ -4800,23 +4800,23 @@
       </c>
       <c r="N15" s="2">
         <f t="shared" si="4"/>
-        <v>18.995789544787566</v>
+        <v>41.609694031809987</v>
       </c>
       <c r="O15" s="2">
         <f t="shared" si="5"/>
-        <v>19.662436806257755</v>
+        <v>29.100866881357877</v>
       </c>
       <c r="P15" s="2">
         <f t="shared" si="6"/>
-        <v>1.3309083224999996</v>
+        <v>6.2183352082810002</v>
       </c>
       <c r="Q15" s="2">
         <f t="shared" si="7"/>
-        <v>10.270524758670899</v>
+        <v>15.65704694835461</v>
       </c>
       <c r="R15" s="2">
         <f t="shared" si="8"/>
-        <v>1.1536499999999998</v>
+        <v>2.4936590000000001</v>
       </c>
       <c r="S15">
         <v>4.0966670000000001</v>
@@ -4865,14 +4865,14 @@
         <v>31</v>
       </c>
       <c r="H16">
-        <v>5.3405769999999997</v>
+        <v>4.213533</v>
       </c>
       <c r="I16">
         <v>5.4902660000000001</v>
       </c>
       <c r="J16" s="2">
         <f t="shared" si="0"/>
-        <v>0.14968900000000041</v>
+        <v>1.2767330000000001</v>
       </c>
       <c r="K16" s="2">
         <f t="shared" si="1"/>
@@ -4880,7 +4880,7 @@
       </c>
       <c r="L16" s="2">
         <f t="shared" si="2"/>
-        <v>-4.0775949444444457</v>
+        <v>-5.9567716527777801</v>
       </c>
       <c r="M16" s="2">
         <f t="shared" si="3"/>
@@ -4888,23 +4888,23 @@
       </c>
       <c r="N16" s="2">
         <f t="shared" si="4"/>
-        <v>16.626780530958904</v>
+        <v>35.483128523336923</v>
       </c>
       <c r="O16" s="2">
         <f t="shared" si="5"/>
-        <v>21.344220743865773</v>
+        <v>31.18079426965096</v>
       </c>
       <c r="P16" s="2">
         <f t="shared" si="6"/>
-        <v>2.240679672100012E-2</v>
+        <v>1.6300471532890004</v>
       </c>
       <c r="Q16" s="2">
         <f t="shared" si="7"/>
-        <v>15.428445108402009</v>
+        <v>21.902761791494058</v>
       </c>
       <c r="R16" s="2">
         <f t="shared" si="8"/>
-        <v>0.14968900000000041</v>
+        <v>1.2767330000000001</v>
       </c>
       <c r="S16">
         <v>4.0692149999999998</v>
@@ -4932,14 +4932,14 @@
         <v>28</v>
       </c>
       <c r="H17">
-        <v>4.6972199999999997</v>
+        <v>3.3110390000000001</v>
       </c>
       <c r="I17">
         <v>4.6242000000000001</v>
       </c>
       <c r="J17" s="2">
         <f t="shared" si="0"/>
-        <v>-7.3019999999999641E-2</v>
+        <v>1.313161</v>
       </c>
       <c r="K17" s="2">
         <f t="shared" si="1"/>
@@ -4947,7 +4947,7 @@
       </c>
       <c r="L17" s="2">
         <f t="shared" si="2"/>
-        <v>-4.7209519444444457</v>
+        <v>-6.85926565277778</v>
       </c>
       <c r="M17" s="2">
         <f t="shared" si="3"/>
@@ -4955,23 +4955,23 @@
       </c>
       <c r="N17" s="2">
         <f t="shared" si="4"/>
-        <v>22.287387261753793</v>
+        <v>47.049525295376988</v>
       </c>
       <c r="O17" s="2">
         <f t="shared" si="5"/>
-        <v>28.800536817141758</v>
+        <v>41.845486947575736</v>
       </c>
       <c r="P17" s="2">
         <f t="shared" si="6"/>
-        <v>5.3319203999999476E-3</v>
+        <v>1.724391811921</v>
       </c>
       <c r="Q17" s="2">
         <f t="shared" si="7"/>
-        <v>22.982167004120456</v>
+        <v>30.75927681956334</v>
       </c>
       <c r="R17" s="2">
         <f t="shared" si="8"/>
-        <v>7.3019999999999641E-2</v>
+        <v>1.313161</v>
       </c>
       <c r="S17">
         <v>4.3104899999999997</v>
@@ -4999,14 +4999,14 @@
         <v>31</v>
       </c>
       <c r="H18">
-        <v>5.7556729999999998</v>
+        <v>4.7018979999999999</v>
       </c>
       <c r="I18">
         <v>5.5021440000000004</v>
       </c>
       <c r="J18" s="2">
         <f t="shared" si="0"/>
-        <v>-0.25352899999999945</v>
+        <v>0.80024600000000046</v>
       </c>
       <c r="K18" s="2">
         <f t="shared" si="1"/>
@@ -5014,7 +5014,7 @@
       </c>
       <c r="L18" s="2">
         <f t="shared" si="2"/>
-        <v>-3.6624989444444456</v>
+        <v>-5.4684066527777802</v>
       </c>
       <c r="M18" s="2">
         <f t="shared" si="3"/>
@@ -5022,23 +5022,23 @@
       </c>
       <c r="N18" s="2">
         <f t="shared" si="4"/>
-        <v>13.413898518056678</v>
+        <v>29.903471320144284</v>
       </c>
       <c r="O18" s="2">
         <f t="shared" si="5"/>
-        <v>19.12789247871244</v>
+        <v>28.55948795367517</v>
       </c>
       <c r="P18" s="2">
         <f t="shared" si="6"/>
-        <v>6.4276953840999726E-2</v>
+        <v>0.64039366051600077</v>
       </c>
       <c r="Q18" s="2">
         <f t="shared" si="7"/>
-        <v>15.335274861669784</v>
+        <v>21.791723880142666</v>
       </c>
       <c r="R18" s="2">
         <f t="shared" si="8"/>
-        <v>0.25352899999999945</v>
+        <v>0.80024600000000046</v>
       </c>
       <c r="S18">
         <v>4.6696390000000001</v>
@@ -5066,14 +5066,14 @@
         <v>30</v>
       </c>
       <c r="H19">
-        <v>5.8229920000000002</v>
+        <v>4.7580549999999997</v>
       </c>
       <c r="I19">
         <v>6.2522029999999997</v>
       </c>
       <c r="J19" s="2">
         <f t="shared" si="0"/>
-        <v>0.42921099999999957</v>
+        <v>1.494148</v>
       </c>
       <c r="K19" s="2">
         <f t="shared" si="1"/>
@@ -5081,7 +5081,7 @@
       </c>
       <c r="L19" s="2">
         <f t="shared" si="2"/>
-        <v>-3.5951799444444452</v>
+        <v>-5.4122496527777804</v>
       </c>
       <c r="M19" s="2">
         <f t="shared" si="3"/>
@@ -5089,23 +5089,23 @@
       </c>
       <c r="N19" s="2">
         <f t="shared" si="4"/>
-        <v>12.925318832935565</v>
+        <v>29.292446303993206</v>
       </c>
       <c r="O19" s="2">
         <f t="shared" si="5"/>
-        <v>16.079712888751647</v>
+        <v>24.206693919005115</v>
       </c>
       <c r="P19" s="2">
         <f t="shared" si="6"/>
-        <v>0.18422208252099961</v>
+        <v>2.2324782459040002</v>
       </c>
       <c r="Q19" s="2">
         <f t="shared" si="7"/>
-        <v>10.023359357186678</v>
+        <v>15.351520561499974</v>
       </c>
       <c r="R19" s="2">
         <f t="shared" si="8"/>
-        <v>0.42921099999999957</v>
+        <v>1.494148</v>
       </c>
       <c r="S19">
         <v>5.725752</v>
@@ -5136,14 +5136,14 @@
         <v>31</v>
       </c>
       <c r="H20">
-        <v>8.1870809999999992</v>
+        <v>8.2818780000000007</v>
       </c>
       <c r="I20">
         <v>7.5640549999999998</v>
       </c>
       <c r="J20" s="2">
         <f t="shared" si="0"/>
-        <v>-0.62302599999999941</v>
+        <v>-0.71782300000000099</v>
       </c>
       <c r="K20" s="2">
         <f t="shared" si="1"/>
@@ -5151,7 +5151,7 @@
       </c>
       <c r="L20" s="2">
         <f t="shared" si="2"/>
-        <v>-1.2310909444444462</v>
+        <v>-1.8884266527777793</v>
       </c>
       <c r="M20" s="2">
         <f t="shared" si="3"/>
@@ -5159,23 +5159,23 @@
       </c>
       <c r="N20" s="2">
         <f t="shared" si="4"/>
-        <v>1.5155849134931185</v>
+        <v>3.5661552229214877</v>
       </c>
       <c r="O20" s="2">
         <f t="shared" si="5"/>
-        <v>3.8911377880685021</v>
+        <v>5.9687940535825481</v>
       </c>
       <c r="P20" s="2">
         <f t="shared" si="6"/>
-        <v>0.38816139667599925</v>
+        <v>0.51526985932900138</v>
       </c>
       <c r="Q20" s="2">
         <f t="shared" si="7"/>
-        <v>3.4377496436760073</v>
+        <v>6.7925372526043004</v>
       </c>
       <c r="R20" s="2">
         <f t="shared" si="8"/>
-        <v>0.62302599999999941</v>
+        <v>0.71782300000000099</v>
       </c>
       <c r="S20">
         <v>6.651535</v>
@@ -5209,14 +5209,14 @@
         <v>30</v>
       </c>
       <c r="H21">
-        <v>11.771432000000001</v>
+        <v>13.595072999999999</v>
       </c>
       <c r="I21">
         <v>10.631712</v>
       </c>
       <c r="J21" s="2">
         <f t="shared" si="0"/>
-        <v>-1.1397200000000005</v>
+        <v>-2.963360999999999</v>
       </c>
       <c r="K21" s="2">
         <f t="shared" si="1"/>
@@ -5224,7 +5224,7 @@
       </c>
       <c r="L21" s="2">
         <f t="shared" si="2"/>
-        <v>2.3532600555555554</v>
+        <v>3.4247683472222192</v>
       </c>
       <c r="M21" s="2">
         <f t="shared" si="3"/>
@@ -5232,23 +5232,23 @@
       </c>
       <c r="N21" s="2">
         <f t="shared" si="4"/>
-        <v>5.5378328890733357</v>
+        <v>11.729038232135212</v>
       </c>
       <c r="O21" s="2">
         <f t="shared" si="5"/>
-        <v>-0.21900912132950826</v>
+        <v>-0.3187303947608876</v>
       </c>
       <c r="P21" s="2">
         <f t="shared" si="6"/>
-        <v>1.2989616784000011</v>
+        <v>8.7815084163209942</v>
       </c>
       <c r="Q21" s="2">
         <f t="shared" si="7"/>
-        <v>1.4726794664377791</v>
+        <v>0.21289674007064649</v>
       </c>
       <c r="R21" s="2">
         <f t="shared" si="8"/>
-        <v>1.1397200000000005</v>
+        <v>2.963360999999999</v>
       </c>
       <c r="S21">
         <v>8.1925410000000003</v>
@@ -5282,14 +5282,14 @@
         <v>31</v>
       </c>
       <c r="H22">
-        <v>13.539778999999999</v>
+        <v>16.21734</v>
       </c>
       <c r="I22">
         <v>16.250326000000001</v>
       </c>
       <c r="J22" s="2">
         <f t="shared" si="0"/>
-        <v>2.7105470000000018</v>
+        <v>3.298600000000107E-2</v>
       </c>
       <c r="K22" s="2">
         <f t="shared" si="1"/>
@@ -5297,7 +5297,7 @@
       </c>
       <c r="L22" s="2">
         <f t="shared" si="2"/>
-        <v>4.121607055555554</v>
+        <v>6.04703534722222</v>
       </c>
       <c r="M22" s="2">
         <f t="shared" si="3"/>
@@ -5305,23 +5305,23 @@
       </c>
       <c r="N22" s="2">
         <f t="shared" si="4"/>
-        <v>16.987644720405324</v>
+        <v>36.566636490554956</v>
       </c>
       <c r="O22" s="2">
         <f t="shared" si="5"/>
-        <v>22.77413653496459</v>
+        <v>33.413182473027625</v>
       </c>
       <c r="P22" s="2">
         <f t="shared" si="6"/>
-        <v>7.34706503920901</v>
+        <v>1.0880761960000707E-3</v>
       </c>
       <c r="Q22" s="2">
         <f t="shared" si="7"/>
-        <v>46.678329038844225</v>
+        <v>36.966659582677913</v>
       </c>
       <c r="R22" s="2">
         <f t="shared" si="8"/>
-        <v>2.7105470000000018</v>
+        <v>3.298600000000107E-2</v>
       </c>
       <c r="S22">
         <v>10.529388000000001</v>
@@ -5355,14 +5355,14 @@
         <v>31</v>
       </c>
       <c r="H23">
-        <v>14.614145000000001</v>
+        <v>17.771920999999999</v>
       </c>
       <c r="I23">
         <v>19.721518</v>
       </c>
       <c r="J23" s="2">
         <f t="shared" si="0"/>
-        <v>5.1073729999999991</v>
+        <v>1.9495970000000007</v>
       </c>
       <c r="K23" s="2">
         <f t="shared" si="1"/>
@@ -5370,7 +5370,7 @@
       </c>
       <c r="L23" s="2">
         <f t="shared" si="2"/>
-        <v>5.1959730555555552</v>
+        <v>7.6016163472222189</v>
       </c>
       <c r="M23" s="2">
         <f t="shared" si="3"/>
@@ -5378,23 +5378,23 @@
       </c>
       <c r="N23" s="2">
         <f t="shared" si="4"/>
-        <v>26.998135994059332</v>
+        <v>57.784571090356067</v>
       </c>
       <c r="O23" s="2">
         <f t="shared" si="5"/>
-        <v>46.746817256679343</v>
+        <v>68.389763849725952</v>
       </c>
       <c r="P23" s="2">
         <f t="shared" si="6"/>
-        <v>26.085258961128989</v>
+        <v>3.8009284624090025</v>
       </c>
       <c r="Q23" s="2">
         <f t="shared" si="7"/>
-        <v>106.15893994053219</v>
+        <v>91.225676404155877</v>
       </c>
       <c r="R23" s="2">
         <f t="shared" si="8"/>
-        <v>5.1073729999999991</v>
+        <v>1.9495970000000007</v>
       </c>
       <c r="S23">
         <v>12.893722</v>
@@ -5428,14 +5428,14 @@
         <v>30</v>
       </c>
       <c r="H24">
-        <v>14.221209</v>
+        <v>17.381886000000002</v>
       </c>
       <c r="I24">
         <v>17.337859999999999</v>
       </c>
       <c r="J24" s="2">
         <f t="shared" si="0"/>
-        <v>3.1166509999999992</v>
+        <v>-4.4026000000002341E-2</v>
       </c>
       <c r="K24" s="2">
         <f t="shared" si="1"/>
@@ -5443,7 +5443,7 @@
       </c>
       <c r="L24" s="2">
         <f t="shared" si="2"/>
-        <v>4.8030370555555546</v>
+        <v>7.2115813472222214</v>
       </c>
       <c r="M24" s="2">
         <f t="shared" si="3"/>
@@ -5451,23 +5451,23 @@
       </c>
       <c r="N24" s="2">
         <f t="shared" si="4"/>
-        <v>23.069164957039771</v>
+        <v>52.006905527603472</v>
       </c>
       <c r="O24" s="2">
         <f t="shared" si="5"/>
-        <v>31.762876629959333</v>
+        <v>47.690776895794848</v>
       </c>
       <c r="P24" s="2">
         <f t="shared" si="6"/>
-        <v>9.7135134558009941</v>
+        <v>1.9382886760002061E-3</v>
       </c>
       <c r="Q24" s="2">
         <f t="shared" si="7"/>
-        <v>62.721458897309311</v>
+        <v>51.373849655493828</v>
       </c>
       <c r="R24" s="2">
         <f t="shared" si="8"/>
-        <v>3.1166509999999992</v>
+        <v>4.4026000000002341E-2</v>
       </c>
       <c r="S24">
         <v>13.478433000000001</v>
@@ -5501,14 +5501,14 @@
         <v>31</v>
       </c>
       <c r="H25">
-        <v>9.4169959999999993</v>
+        <v>10.232779000000001</v>
       </c>
       <c r="I25">
         <v>11.302659</v>
       </c>
       <c r="J25" s="2">
         <f t="shared" si="0"/>
-        <v>1.885663000000001</v>
+        <v>1.0698799999999995</v>
       </c>
       <c r="K25" s="2">
         <f t="shared" si="1"/>
@@ -5516,7 +5516,7 @@
       </c>
       <c r="L25" s="2">
         <f t="shared" si="2"/>
-        <v>-1.1759444444461309E-3</v>
+        <v>6.2474347222220672E-2</v>
       </c>
       <c r="M25" s="2">
         <f t="shared" si="3"/>
@@ -5524,23 +5524,23 @@
       </c>
       <c r="N25" s="2">
         <f t="shared" si="4"/>
-        <v>1.3828453364237194E-6</v>
+        <v>3.9030440608425919E-3</v>
       </c>
       <c r="O25" s="2">
         <f t="shared" si="5"/>
-        <v>-6.7955564118230482E-4</v>
+        <v>3.6102721760838202E-2</v>
       </c>
       <c r="P25" s="2">
         <f t="shared" si="6"/>
-        <v>3.5557249495690035</v>
+        <v>1.1446432143999989</v>
       </c>
       <c r="Q25" s="2">
         <f t="shared" si="7"/>
-        <v>3.5512914625564447</v>
+        <v>1.2822263676730603</v>
       </c>
       <c r="R25" s="2">
         <f t="shared" si="8"/>
-        <v>1.885663000000001</v>
+        <v>1.0698799999999995</v>
       </c>
       <c r="S25">
         <v>12.416278</v>
@@ -5574,14 +5574,14 @@
         <v>30</v>
       </c>
       <c r="H26">
-        <v>5.7774590000000003</v>
+        <v>4.8344560000000003</v>
       </c>
       <c r="I26">
         <v>6.5582289999999999</v>
       </c>
       <c r="J26" s="2">
         <f t="shared" si="0"/>
-        <v>0.78076999999999952</v>
+        <v>1.7237729999999996</v>
       </c>
       <c r="K26" s="2">
         <f t="shared" si="1"/>
@@ -5589,7 +5589,7 @@
       </c>
       <c r="L26" s="2">
         <f t="shared" si="2"/>
-        <v>-3.640712944444445</v>
+        <v>-5.3358486527777798</v>
       </c>
       <c r="M26" s="2">
         <f t="shared" si="3"/>
@@ -5597,23 +5597,23 @@
       </c>
       <c r="N26" s="2">
         <f t="shared" si="4"/>
-        <v>13.254790743845341</v>
+        <v>28.471280845350446</v>
       </c>
       <c r="O26" s="2">
         <f t="shared" si="5"/>
-        <v>15.169209838705743</v>
+        <v>22.232076276453764</v>
       </c>
       <c r="P26" s="2">
         <f t="shared" si="6"/>
-        <v>0.60960179289999927</v>
+        <v>2.9713933555289986</v>
       </c>
       <c r="Q26" s="2">
         <f t="shared" si="7"/>
-        <v>8.179273645477565</v>
+        <v>13.047090521390027</v>
       </c>
       <c r="R26" s="2">
         <f t="shared" si="8"/>
-        <v>0.78076999999999952</v>
+        <v>1.7237729999999996</v>
       </c>
       <c r="S26">
         <v>7.2547030000000001</v>
@@ -5647,14 +5647,14 @@
         <v>31</v>
       </c>
       <c r="H27">
-        <v>5.1599469999999998</v>
+        <v>4.0301580000000001</v>
       </c>
       <c r="I27">
         <v>3.8962509999999999</v>
       </c>
       <c r="J27" s="2">
         <f t="shared" si="0"/>
-        <v>-1.2636959999999999</v>
+        <v>-0.13390700000000022</v>
       </c>
       <c r="K27" s="2">
         <f t="shared" si="1"/>
@@ -5662,7 +5662,7 @@
       </c>
       <c r="L27" s="2">
         <f t="shared" si="2"/>
-        <v>-4.2582249444444455</v>
+        <v>-6.1401466527777799</v>
       </c>
       <c r="M27" s="2">
         <f t="shared" si="3"/>
@@ -5670,23 +5670,23 @@
       </c>
       <c r="N27" s="2">
         <f t="shared" si="4"/>
-        <v>18.132479677488902</v>
+        <v>37.701400917618173</v>
       </c>
       <c r="O27" s="2">
         <f t="shared" si="5"/>
-        <v>29.077405128910637</v>
+        <v>41.928158822769163</v>
       </c>
       <c r="P27" s="2">
         <f t="shared" si="6"/>
-        <v>1.5969275804159999</v>
+        <v>1.7931084649000058E-2</v>
       </c>
       <c r="Q27" s="2">
         <f t="shared" si="7"/>
-        <v>30.491610916694242</v>
+        <v>39.363749237934215</v>
       </c>
       <c r="R27" s="2">
         <f t="shared" si="8"/>
-        <v>1.2636959999999999</v>
+        <v>0.13390700000000022</v>
       </c>
       <c r="S27">
         <v>3.306524</v>
@@ -5720,14 +5720,14 @@
         <v>31</v>
       </c>
       <c r="H28">
-        <v>4.8252810000000004</v>
+        <v>3.4191470000000002</v>
       </c>
       <c r="I28">
         <v>4.9214390000000003</v>
       </c>
       <c r="J28" s="2">
         <f t="shared" si="0"/>
-        <v>9.6157999999999966E-2</v>
+        <v>1.5022920000000002</v>
       </c>
       <c r="K28" s="2">
         <f t="shared" si="1"/>
@@ -5735,7 +5735,7 @@
       </c>
       <c r="L28" s="2">
         <f t="shared" si="2"/>
-        <v>-4.592890944444445</v>
+        <v>-6.7511576527777795</v>
       </c>
       <c r="M28" s="2">
         <f t="shared" si="3"/>
@@ -5743,23 +5743,23 @@
       </c>
       <c r="N28" s="2">
         <f t="shared" si="4"/>
-        <v>21.094647227559786</v>
+        <v>45.578129652659975</v>
       </c>
       <c r="O28" s="2">
         <f t="shared" si="5"/>
-        <v>26.654104352654155</v>
+        <v>39.179258283069217</v>
       </c>
       <c r="P28" s="2">
         <f t="shared" si="6"/>
-        <v>9.246360963999993E-3</v>
+        <v>2.2568812532640004</v>
       </c>
       <c r="Q28" s="2">
         <f t="shared" si="7"/>
-        <v>20.220607173652009</v>
+        <v>27.550590640910308</v>
       </c>
       <c r="R28" s="2">
         <f t="shared" si="8"/>
-        <v>9.6157999999999966E-2</v>
+        <v>1.5022920000000002</v>
       </c>
       <c r="S28">
         <v>4.1439440000000003</v>
@@ -5793,14 +5793,14 @@
         <v>29</v>
       </c>
       <c r="H29">
-        <v>5.2225970000000004</v>
+        <v>3.9419179999999998</v>
       </c>
       <c r="I29">
         <v>5.1279089999999998</v>
       </c>
       <c r="J29" s="2">
         <f t="shared" si="0"/>
-        <v>-9.468800000000055E-2</v>
+        <v>1.185991</v>
       </c>
       <c r="K29" s="2">
         <f t="shared" si="1"/>
@@ -5808,7 +5808,7 @@
       </c>
       <c r="L29" s="2">
         <f t="shared" si="2"/>
-        <v>-4.195574944444445</v>
+        <v>-6.2283866527777807</v>
       </c>
       <c r="M29" s="2">
         <f t="shared" si="3"/>
@@ -5816,23 +5816,23 @@
       </c>
       <c r="N29" s="2">
         <f t="shared" si="4"/>
-        <v>17.602849114450009</v>
+        <v>38.79280029650041</v>
       </c>
       <c r="O29" s="2">
         <f t="shared" si="5"/>
-        <v>23.482084450903436</v>
+        <v>34.859465820547747</v>
       </c>
       <c r="P29" s="2">
         <f t="shared" si="6"/>
-        <v>8.9658173440001036E-3</v>
+        <v>1.4065746520810001</v>
       </c>
       <c r="Q29" s="2">
         <f t="shared" si="7"/>
-        <v>18.406356132473125</v>
+        <v>25.425753919152257</v>
       </c>
       <c r="R29" s="2">
         <f t="shared" si="8"/>
-        <v>9.468800000000055E-2</v>
+        <v>1.185991</v>
       </c>
       <c r="S29">
         <v>4.8668040000000001</v>
@@ -5866,14 +5866,14 @@
         <v>31</v>
       </c>
       <c r="H30">
-        <v>4.6455700000000002</v>
+        <v>3.101648</v>
       </c>
       <c r="I30">
         <v>5.0719139999999996</v>
       </c>
       <c r="J30" s="2">
         <f t="shared" si="0"/>
-        <v>0.42634399999999939</v>
+        <v>1.9702659999999996</v>
       </c>
       <c r="K30" s="2">
         <f t="shared" si="1"/>
@@ -5881,7 +5881,7 @@
       </c>
       <c r="L30" s="2">
         <f t="shared" si="2"/>
-        <v>-4.7726019444444452</v>
+        <v>-7.0686566527777801</v>
       </c>
       <c r="M30" s="2">
         <f t="shared" si="3"/>
@@ -5889,23 +5889,23 @@
       </c>
       <c r="N30" s="2">
         <f t="shared" si="4"/>
-        <v>22.777729320114901</v>
+        <v>49.96590687485957</v>
       </c>
       <c r="O30" s="2">
         <f t="shared" si="5"/>
-        <v>26.978870977516618</v>
+        <v>39.958156586187947</v>
       </c>
       <c r="P30" s="2">
         <f t="shared" si="6"/>
-        <v>0.18176920633599947</v>
+        <v>3.8819481107559985</v>
       </c>
       <c r="Q30" s="2">
         <f t="shared" si="7"/>
-        <v>18.889958119646458</v>
+        <v>25.993587248331842</v>
       </c>
       <c r="R30" s="2">
         <f t="shared" si="8"/>
-        <v>0.42634399999999939</v>
+        <v>1.9702659999999996</v>
       </c>
       <c r="S30">
         <v>4.7258519999999997</v>
@@ -5939,14 +5939,14 @@
         <v>30</v>
       </c>
       <c r="H31">
-        <v>8.1837680000000006</v>
+        <v>8.2963290000000001</v>
       </c>
       <c r="I31">
         <v>6.5960349999999996</v>
       </c>
       <c r="J31" s="2">
         <f t="shared" si="0"/>
-        <v>-1.5877330000000009</v>
+        <v>-1.7002940000000004</v>
       </c>
       <c r="K31" s="2">
         <f t="shared" si="1"/>
@@ -5954,7 +5954,7 @@
       </c>
       <c r="L31" s="2">
         <f t="shared" si="2"/>
-        <v>-1.2344039444444448</v>
+        <v>-1.87397565277778</v>
       </c>
       <c r="M31" s="2">
         <f t="shared" si="3"/>
@@ -5962,23 +5962,23 @@
       </c>
       <c r="N31" s="2">
         <f t="shared" si="4"/>
-        <v>1.523753098060004</v>
+        <v>3.5117847472039068</v>
       </c>
       <c r="O31" s="2">
         <f t="shared" si="5"/>
-        <v>5.0965369705428731</v>
+        <v>7.7371643530980387</v>
       </c>
       <c r="P31" s="2">
         <f t="shared" si="6"/>
-        <v>2.5208960792890029</v>
+        <v>2.8909996864360012</v>
       </c>
       <c r="Q31" s="2">
         <f t="shared" si="7"/>
-        <v>7.9644569331982327</v>
+        <v>12.775403550768194</v>
       </c>
       <c r="R31" s="2">
         <f t="shared" si="8"/>
-        <v>1.5877330000000009</v>
+        <v>1.7002940000000004</v>
       </c>
       <c r="S31">
         <v>5.8077240000000003</v>
@@ -6012,14 +6012,14 @@
         <v>31</v>
       </c>
       <c r="H32">
-        <v>9.8008500000000005</v>
+        <v>10.669551999999999</v>
       </c>
       <c r="I32">
         <v>8.7931030000000003</v>
       </c>
       <c r="J32" s="2">
         <f t="shared" si="0"/>
-        <v>-1.0077470000000002</v>
+        <v>-1.8764489999999991</v>
       </c>
       <c r="K32" s="2">
         <f t="shared" si="1"/>
@@ -6027,7 +6027,7 @@
       </c>
       <c r="L32" s="2">
         <f t="shared" si="2"/>
-        <v>0.38267805555555512</v>
+        <v>0.49924734722221942</v>
       </c>
       <c r="M32" s="2">
         <f t="shared" si="3"/>
@@ -6035,23 +6035,23 @@
       </c>
       <c r="N32" s="2">
         <f t="shared" si="4"/>
-        <v>0.14644249420378053</v>
+        <v>0.24924791370842331</v>
       </c>
       <c r="O32" s="2">
         <f t="shared" si="5"/>
-        <v>-0.73920973394976275</v>
+        <v>-0.96438375119130704</v>
       </c>
       <c r="P32" s="2">
         <f t="shared" si="6"/>
-        <v>1.0155540160090004</v>
+        <v>3.521060849600997</v>
       </c>
       <c r="Q32" s="2">
         <f t="shared" si="7"/>
-        <v>0.39071118530889276</v>
+        <v>1.8966843924138481</v>
       </c>
       <c r="R32" s="2">
         <f t="shared" si="8"/>
-        <v>1.0077470000000002</v>
+        <v>1.8764489999999991</v>
       </c>
       <c r="S32">
         <v>7.3342520000000002</v>
@@ -6079,14 +6079,14 @@
         <v>30</v>
       </c>
       <c r="H33">
-        <v>10.984868000000001</v>
+        <v>12.462146000000001</v>
       </c>
       <c r="I33">
         <v>11.085842</v>
       </c>
       <c r="J33" s="2">
         <f t="shared" si="0"/>
-        <v>0.10097399999999901</v>
+        <v>-1.3763040000000011</v>
       </c>
       <c r="K33" s="2">
         <f t="shared" si="1"/>
@@ -6094,7 +6094,7 @@
       </c>
       <c r="L33" s="2">
         <f t="shared" si="2"/>
-        <v>1.5666960555555551</v>
+        <v>2.2918413472222205</v>
       </c>
       <c r="M33" s="2">
         <f t="shared" si="3"/>
@@ -6102,23 +6102,23 @@
       </c>
       <c r="N33" s="2">
         <f t="shared" si="4"/>
-        <v>2.4545365304933351</v>
+        <v>5.252536760837363</v>
       </c>
       <c r="O33" s="2">
         <f t="shared" si="5"/>
-        <v>0.56567713116943275</v>
+        <v>0.82750079940198173</v>
       </c>
       <c r="P33" s="2">
         <f t="shared" si="6"/>
-        <v>1.0195748675999801E-2</v>
+        <v>1.894212700416003</v>
       </c>
       <c r="Q33" s="2">
         <f t="shared" si="7"/>
-        <v>2.781123414196665</v>
+        <v>0.83820863415869884</v>
       </c>
       <c r="R33" s="2">
         <f t="shared" si="8"/>
-        <v>0.10097399999999901</v>
+        <v>1.3763040000000011</v>
       </c>
       <c r="S33">
         <v>8.6606909999999999</v>
@@ -6146,14 +6146,14 @@
         <v>31</v>
       </c>
       <c r="H34">
-        <v>14.640597</v>
+        <v>17.817267999999999</v>
       </c>
       <c r="I34">
         <v>17.259895</v>
       </c>
       <c r="J34" s="2">
         <f t="shared" si="0"/>
-        <v>2.6192980000000006</v>
+        <v>-0.55737299999999834</v>
       </c>
       <c r="K34" s="2">
         <f t="shared" si="1"/>
@@ -6161,7 +6161,7 @@
       </c>
       <c r="L34" s="2">
         <f t="shared" si="2"/>
-        <v>5.2224250555555543</v>
+        <v>7.6469633472222185</v>
       </c>
       <c r="M34" s="2">
         <f t="shared" si="3"/>
@@ -6169,23 +6169,23 @@
       </c>
       <c r="N34" s="2">
         <f t="shared" si="4"/>
-        <v>27.273723460894434</v>
+        <v>58.476048433760035</v>
       </c>
       <c r="O34" s="2">
         <f t="shared" si="5"/>
-        <v>34.129157383647119</v>
+        <v>49.973798150860183</v>
       </c>
       <c r="P34" s="2">
         <f t="shared" si="6"/>
-        <v>6.8607220128040032</v>
+        <v>0.31066466112899815</v>
       </c>
       <c r="Q34" s="2">
         <f t="shared" si="7"/>
-        <v>61.492620480031547</v>
+        <v>50.262291291426479</v>
       </c>
       <c r="R34" s="2">
         <f t="shared" si="8"/>
-        <v>2.6192980000000006</v>
+        <v>0.55737299999999834</v>
       </c>
       <c r="S34">
         <v>11.135647000000001</v>
@@ -6213,14 +6213,14 @@
         <v>31</v>
       </c>
       <c r="H35">
-        <v>15.450846</v>
+        <v>18.962933</v>
       </c>
       <c r="I35">
         <v>20.230844000000001</v>
       </c>
       <c r="J35" s="2">
         <f t="shared" si="0"/>
-        <v>4.7799980000000009</v>
+        <v>1.2679110000000016</v>
       </c>
       <c r="K35" s="2">
         <f t="shared" si="1"/>
@@ -6228,7 +6228,7 @@
       </c>
       <c r="L35" s="2">
         <f t="shared" si="2"/>
-        <v>6.0326740555555549</v>
+        <v>8.7926283472222195</v>
       </c>
       <c r="M35" s="2">
         <f t="shared" si="3"/>
@@ -6236,23 +6236,23 @@
       </c>
       <c r="N35" s="2">
         <f t="shared" si="4"/>
-        <v>36.393156260573107</v>
+        <v>77.310313252375735</v>
       </c>
       <c r="O35" s="2">
         <f t="shared" si="5"/>
-        <v>57.346996136643142</v>
+        <v>83.583303061888444</v>
       </c>
       <c r="P35" s="2">
         <f t="shared" si="6"/>
-        <v>22.848380880004008</v>
+        <v>1.607598303921004</v>
       </c>
       <c r="Q35" s="2">
         <f t="shared" si="7"/>
-        <v>116.91387698099201</v>
+        <v>101.21445195700652</v>
       </c>
       <c r="R35" s="2">
         <f t="shared" si="8"/>
-        <v>4.7799980000000009</v>
+        <v>1.2679110000000016</v>
       </c>
       <c r="S35">
         <v>13.613049999999999</v>
@@ -6280,14 +6280,14 @@
         <v>30</v>
       </c>
       <c r="H36">
-        <v>13.818787</v>
+        <v>16.609960999999998</v>
       </c>
       <c r="I36">
         <v>16.425416999999999</v>
       </c>
       <c r="J36" s="2">
         <f t="shared" si="0"/>
-        <v>2.6066299999999991</v>
+        <v>-0.18454399999999893</v>
       </c>
       <c r="K36" s="2">
         <f t="shared" si="1"/>
@@ -6295,7 +6295,7 @@
       </c>
       <c r="L36" s="2">
         <f t="shared" si="2"/>
-        <v>4.400615055555555</v>
+        <v>6.4396563472222184</v>
       </c>
       <c r="M36" s="2">
         <f t="shared" si="3"/>
@@ -6303,23 +6303,23 @@
       </c>
       <c r="N36" s="2">
         <f t="shared" si="4"/>
-        <v>19.365412867182219</v>
+        <v>41.469173870319402</v>
       </c>
       <c r="O36" s="2">
         <f t="shared" si="5"/>
-        <v>25.086316648413753</v>
+        <v>36.710154420218771</v>
       </c>
       <c r="P36" s="2">
         <f t="shared" si="6"/>
-        <v>6.794519956899995</v>
+        <v>3.4056487935999608E-2</v>
       </c>
       <c r="Q36" s="2">
         <f t="shared" si="7"/>
-        <v>49.101483268607758</v>
+        <v>39.126430476371866</v>
       </c>
       <c r="R36" s="2">
         <f t="shared" si="8"/>
-        <v>2.6066299999999991</v>
+        <v>0.18454399999999893</v>
       </c>
       <c r="S36">
         <v>13.893703</v>
@@ -6347,14 +6347,14 @@
         <v>31</v>
       </c>
       <c r="H37">
-        <v>9.8301639999999999</v>
+        <v>10.76773</v>
       </c>
       <c r="I37">
         <v>10.409481</v>
       </c>
       <c r="J37" s="2">
         <f t="shared" si="0"/>
-        <v>0.57931699999999964</v>
+        <v>-0.35824900000000071</v>
       </c>
       <c r="K37" s="2">
         <f t="shared" si="1"/>
@@ -6362,7 +6362,7 @@
       </c>
       <c r="L37" s="2">
         <f t="shared" si="2"/>
-        <v>0.41199205555555451</v>
+        <v>0.59742534722222018</v>
       </c>
       <c r="M37" s="2">
         <f t="shared" si="3"/>
@@ -6370,23 +6370,23 @@
       </c>
       <c r="N37" s="2">
         <f t="shared" si="4"/>
-        <v>0.16973745384089112</v>
+        <v>0.35691704550359032</v>
       </c>
       <c r="O37" s="2">
         <f t="shared" si="5"/>
-        <v>-0.12989996786062463</v>
+        <v>-0.18836657735703424</v>
       </c>
       <c r="P37" s="2">
         <f t="shared" si="6"/>
-        <v>0.33560818648899959</v>
+        <v>0.1283423460010005</v>
       </c>
       <c r="Q37" s="2">
         <f t="shared" si="7"/>
-        <v>0.98269364362644473</v>
+        <v>5.7205325070563695E-2</v>
       </c>
       <c r="R37" s="2">
         <f t="shared" si="8"/>
-        <v>0.57931699999999964</v>
+        <v>0.35824900000000071</v>
       </c>
       <c r="S37">
         <v>12.509562000000001</v>
@@ -6414,14 +6414,14 @@
         <v>30</v>
       </c>
       <c r="H38">
-        <v>7.1806229999999998</v>
+        <v>6.8409709999999997</v>
       </c>
       <c r="I38">
         <v>8.1149190000000004</v>
       </c>
       <c r="J38" s="2">
         <f t="shared" si="0"/>
-        <v>0.93429600000000068</v>
+        <v>1.2739480000000007</v>
       </c>
       <c r="K38" s="2">
         <f t="shared" si="1"/>
@@ -6429,7 +6429,7 @@
       </c>
       <c r="L38" s="2">
         <f t="shared" si="2"/>
-        <v>-2.2375489444444456</v>
+        <v>-3.3293336527777804</v>
       </c>
       <c r="M38" s="2">
         <f t="shared" si="3"/>
@@ -6437,23 +6437,23 @@
       </c>
       <c r="N38" s="2">
         <f t="shared" si="4"/>
-        <v>5.006625278784453</v>
+        <v>11.084462571518637</v>
       </c>
       <c r="O38" s="2">
         <f t="shared" si="5"/>
-        <v>5.8396878410631343</v>
+        <v>8.6890922762791138</v>
       </c>
       <c r="P38" s="2">
         <f t="shared" si="6"/>
-        <v>0.87290901561600132</v>
+        <v>1.6229435067040019</v>
       </c>
       <c r="Q38" s="2">
         <f t="shared" si="7"/>
-        <v>1.6984682372031155</v>
+        <v>4.2246101816447394</v>
       </c>
       <c r="R38" s="2">
         <f t="shared" si="8"/>
-        <v>0.93429600000000068</v>
+        <v>1.2739480000000007</v>
       </c>
       <c r="S38">
         <v>6.3092430000000004</v>
@@ -6481,14 +6481,14 @@
         <v>31</v>
       </c>
       <c r="H39">
-        <v>4.2529050000000002</v>
+        <v>2.559825</v>
       </c>
       <c r="I39">
         <v>6.1558140000000003</v>
       </c>
       <c r="J39" s="2">
         <f t="shared" si="0"/>
-        <v>1.9029090000000002</v>
+        <v>3.5959890000000003</v>
       </c>
       <c r="K39" s="2">
         <f t="shared" si="1"/>
@@ -6496,7 +6496,7 @@
       </c>
       <c r="L39" s="2">
         <f t="shared" si="2"/>
-        <v>-5.1652669444444452</v>
+        <v>-7.61047965277778</v>
       </c>
       <c r="M39" s="2">
         <f t="shared" si="3"/>
@@ -6504,23 +6504,23 @@
       </c>
       <c r="N39" s="2">
         <f t="shared" si="4"/>
-        <v>26.679982607370455</v>
+        <v>57.919400545344601</v>
       </c>
       <c r="O39" s="2">
         <f t="shared" si="5"/>
-        <v>23.59992008261321</v>
+        <v>34.772009564595173</v>
       </c>
       <c r="P39" s="2">
         <f t="shared" si="6"/>
-        <v>3.6210626622810005</v>
+        <v>12.931136888121003</v>
       </c>
       <c r="Q39" s="2">
         <f t="shared" si="7"/>
-        <v>10.642979357679785</v>
+        <v>16.116135201240162</v>
       </c>
       <c r="R39" s="2">
         <f t="shared" si="8"/>
-        <v>1.9029090000000002</v>
+        <v>3.5959890000000003</v>
       </c>
       <c r="S39">
         <v>4.0317879999999997</v>
@@ -6548,14 +6548,14 @@
         <v>31</v>
       </c>
       <c r="H40">
-        <v>4.5596059999999996</v>
+        <v>3.1383709999999998</v>
       </c>
       <c r="I40">
         <v>4.3148499999999999</v>
       </c>
       <c r="J40" s="2">
         <f t="shared" ref="J40:J75" si="10">I40-H40</f>
-        <v>-0.24475599999999975</v>
+        <v>1.1764790000000001</v>
       </c>
       <c r="K40" s="2">
         <f t="shared" ref="K40:K75" si="11">I40-I$2</f>
@@ -6563,7 +6563,7 @@
       </c>
       <c r="L40" s="2">
         <f t="shared" ref="L40:L75" si="12">H40-H$2</f>
-        <v>-4.8585659444444458</v>
+        <v>-7.0319336527777807</v>
       </c>
       <c r="M40" s="2">
         <f t="shared" ref="M40:M75" si="13">K40*K40</f>
@@ -6571,23 +6571,23 @@
       </c>
       <c r="N40" s="2">
         <f t="shared" ref="N40:N75" si="14">L40*L40</f>
-        <v>23.605663036515349</v>
+        <v>49.44809089706866</v>
       </c>
       <c r="O40" s="2">
         <f t="shared" ref="O40:O75" si="15">K40*L40</f>
-        <v>31.143059169262454</v>
+        <v>45.074190270731719</v>
       </c>
       <c r="P40" s="2">
         <f t="shared" ref="P40:P75" si="16">J40*J40</f>
-        <v>5.9905499535999877E-2</v>
+        <v>1.384102837441</v>
       </c>
       <c r="Q40" s="2">
         <f t="shared" ref="Q40:Q75" si="17">(I40-H$2)*(I40-H$2)</f>
-        <v>26.043894868648238</v>
+        <v>34.286349190736956</v>
       </c>
       <c r="R40" s="2">
         <f t="shared" ref="R40:R75" si="18">ABS(J40)</f>
-        <v>0.24475599999999975</v>
+        <v>1.1764790000000001</v>
       </c>
       <c r="S40">
         <v>4.3465230000000004</v>
@@ -6615,14 +6615,14 @@
         <v>28</v>
       </c>
       <c r="H41">
-        <v>4.6835370000000003</v>
+        <v>3.2248890000000001</v>
       </c>
       <c r="I41">
         <v>5.3706670000000001</v>
       </c>
       <c r="J41" s="2">
         <f t="shared" si="10"/>
-        <v>0.6871299999999998</v>
+        <v>2.145778</v>
       </c>
       <c r="K41" s="2">
         <f t="shared" si="11"/>
@@ -6630,7 +6630,7 @@
       </c>
       <c r="L41" s="2">
         <f t="shared" si="12"/>
-        <v>-4.7346349444444451</v>
+        <v>-6.9454156527777799</v>
       </c>
       <c r="M41" s="2">
         <f t="shared" si="13"/>
@@ -6638,23 +6638,23 @@
       </c>
       <c r="N41" s="2">
         <f t="shared" si="14"/>
-        <v>22.416768057154453</v>
+        <v>48.238798589850596</v>
       </c>
       <c r="O41" s="2">
         <f t="shared" si="15"/>
-        <v>25.349762286451934</v>
+        <v>37.186528178927695</v>
       </c>
       <c r="P41" s="2">
         <f t="shared" si="16"/>
-        <v>0.47214763689999972</v>
+        <v>4.6043632252839997</v>
       </c>
       <c r="Q41" s="2">
         <f t="shared" si="17"/>
-        <v>16.382296275302231</v>
+        <v>23.036521597962196</v>
       </c>
       <c r="R41" s="2">
         <f t="shared" si="18"/>
-        <v>0.6871299999999998</v>
+        <v>2.145778</v>
       </c>
       <c r="S41">
         <v>5.355829</v>
@@ -6682,14 +6682,14 @@
         <v>31</v>
       </c>
       <c r="H42">
-        <v>6.7431599999999996</v>
+        <v>6.1851079999999996</v>
       </c>
       <c r="I42">
         <v>6.000432</v>
       </c>
       <c r="J42" s="2">
         <f t="shared" si="10"/>
-        <v>-0.74272799999999961</v>
+        <v>-0.18467599999999962</v>
       </c>
       <c r="K42" s="2">
         <f t="shared" si="11"/>
@@ -6697,7 +6697,7 @@
       </c>
       <c r="L42" s="2">
         <f t="shared" si="12"/>
-        <v>-2.6750119444444458</v>
+        <v>-3.9851966527777805</v>
       </c>
       <c r="M42" s="2">
         <f t="shared" si="13"/>
@@ -6705,23 +6705,23 @@
       </c>
       <c r="N42" s="2">
         <f t="shared" si="14"/>
-        <v>7.1556889029204545</v>
+        <v>15.881792361311225</v>
       </c>
       <c r="O42" s="2">
         <f t="shared" si="15"/>
-        <v>12.637682685594262</v>
+        <v>18.827448917413204</v>
       </c>
       <c r="P42" s="2">
         <f t="shared" si="16"/>
-        <v>0.55164488198399941</v>
+        <v>3.4105224975999861E-2</v>
       </c>
       <c r="Q42" s="2">
         <f t="shared" si="17"/>
-        <v>11.680946327851121</v>
+        <v>17.387837940383999</v>
       </c>
       <c r="R42" s="2">
         <f t="shared" si="18"/>
-        <v>0.74272799999999961</v>
+        <v>0.18467599999999962</v>
       </c>
       <c r="S42">
         <v>5.5344850000000001</v>
@@ -6749,14 +6749,14 @@
         <v>30</v>
       </c>
       <c r="H43">
-        <v>7.9069370000000001</v>
+        <v>7.8967999999999998</v>
       </c>
       <c r="I43">
         <v>7.3541650000000001</v>
       </c>
       <c r="J43" s="2">
         <f t="shared" si="10"/>
-        <v>-0.55277200000000004</v>
+        <v>-0.54263499999999976</v>
       </c>
       <c r="K43" s="2">
         <f t="shared" si="11"/>
@@ -6764,7 +6764,7 @@
       </c>
       <c r="L43" s="2">
         <f t="shared" si="12"/>
-        <v>-1.5112349444444453</v>
+        <v>-2.2735046527777802</v>
       </c>
       <c r="M43" s="2">
         <f t="shared" si="13"/>
@@ -6772,23 +6772,23 @@
       </c>
       <c r="N43" s="2">
         <f t="shared" si="14"/>
-        <v>2.2838310573100058</v>
+        <v>5.1688234062022147</v>
       </c>
       <c r="O43" s="2">
         <f t="shared" si="15"/>
-        <v>5.0937885485968319</v>
+        <v>7.6631049381658833</v>
       </c>
       <c r="P43" s="2">
         <f t="shared" si="16"/>
-        <v>0.30555688398400005</v>
+        <v>0.29445274322499976</v>
       </c>
       <c r="Q43" s="2">
         <f t="shared" si="17"/>
-        <v>4.260124666714896</v>
+        <v>7.9306425439473553</v>
       </c>
       <c r="R43" s="2">
         <f t="shared" si="18"/>
-        <v>0.55277200000000004</v>
+        <v>0.54263499999999976</v>
       </c>
       <c r="S43">
         <v>7.4366459999999996</v>
@@ -6816,14 +6816,14 @@
         <v>31</v>
       </c>
       <c r="H44">
-        <v>10.611583</v>
+        <v>11.922974</v>
       </c>
       <c r="I44">
         <v>10.393872</v>
       </c>
       <c r="J44" s="2">
         <f t="shared" si="10"/>
-        <v>-0.21771099999999954</v>
+        <v>-1.529102</v>
       </c>
       <c r="K44" s="2">
         <f t="shared" si="11"/>
@@ -6831,7 +6831,7 @@
       </c>
       <c r="L44" s="2">
         <f t="shared" si="12"/>
-        <v>1.1934110555555542</v>
+        <v>1.7526693472222199</v>
       </c>
       <c r="M44" s="2">
         <f t="shared" si="13"/>
@@ -6839,23 +6839,23 @@
       </c>
       <c r="N44" s="2">
         <f t="shared" si="14"/>
-        <v>1.424229947522222</v>
+        <v>3.0718498406923622</v>
       </c>
       <c r="O44" s="2">
         <f t="shared" si="15"/>
-        <v>-0.3949071936775807</v>
+        <v>-0.57996926552187822</v>
       </c>
       <c r="P44" s="2">
         <f t="shared" si="16"/>
-        <v>4.7398079520999802E-2</v>
+        <v>2.3381529264039997</v>
       </c>
       <c r="Q44" s="2">
         <f t="shared" si="17"/>
-        <v>0.95199059841111233</v>
+        <v>4.9982358743980652E-2</v>
       </c>
       <c r="R44" s="2">
         <f t="shared" si="18"/>
-        <v>0.21771099999999954</v>
+        <v>1.529102</v>
       </c>
       <c r="S44">
         <v>9.1137759999999997</v>
@@ -6883,14 +6883,14 @@
         <v>30</v>
       </c>
       <c r="H45">
-        <v>12.615589</v>
+        <v>14.898326000000001</v>
       </c>
       <c r="I45">
         <v>13.887563999999999</v>
       </c>
       <c r="J45" s="2">
         <f t="shared" si="10"/>
-        <v>1.2719749999999994</v>
+        <v>-1.0107620000000015</v>
       </c>
       <c r="K45" s="2">
         <f t="shared" si="11"/>
@@ -6898,7 +6898,7 @@
       </c>
       <c r="L45" s="2">
         <f t="shared" si="12"/>
-        <v>3.1974170555555546</v>
+        <v>4.7280213472222208</v>
       </c>
       <c r="M45" s="2">
         <f t="shared" si="13"/>
@@ -6906,23 +6906,23 @@
       </c>
       <c r="N45" s="2">
         <f t="shared" si="14"/>
-        <v>10.223475827157552</v>
+        <v>22.354185859789023</v>
       </c>
       <c r="O45" s="2">
         <f t="shared" si="15"/>
-        <v>10.112745055709501</v>
+        <v>14.953718477023287</v>
       </c>
       <c r="P45" s="2">
         <f t="shared" si="16"/>
-        <v>1.6179204006249985</v>
+        <v>1.0216398206440029</v>
       </c>
       <c r="Q45" s="2">
         <f t="shared" si="17"/>
-        <v>19.9754653462631</v>
+        <v>13.81801705451096</v>
       </c>
       <c r="R45" s="2">
         <f t="shared" si="18"/>
-        <v>1.2719749999999994</v>
+        <v>1.0107620000000015</v>
       </c>
       <c r="S45">
         <v>10.387589</v>
@@ -6950,14 +6950,14 @@
         <v>31</v>
       </c>
       <c r="H46">
-        <v>15.329357</v>
+        <v>18.877089000000002</v>
       </c>
       <c r="I46">
         <v>20.018450000000001</v>
       </c>
       <c r="J46" s="2">
         <f t="shared" si="10"/>
-        <v>4.6890930000000015</v>
+        <v>1.1413609999999998</v>
       </c>
       <c r="K46" s="2">
         <f t="shared" si="11"/>
@@ -6965,7 +6965,7 @@
       </c>
       <c r="L46" s="2">
         <f t="shared" si="12"/>
-        <v>5.9111850555555545</v>
+        <v>8.7067843472222215</v>
       </c>
       <c r="M46" s="2">
         <f t="shared" si="13"/>
@@ -6973,23 +6973,23 @@
       </c>
       <c r="N46" s="2">
         <f t="shared" si="14"/>
-        <v>34.942108761023327</v>
+        <v>75.80809366903388</v>
       </c>
       <c r="O46" s="2">
         <f t="shared" si="15"/>
-        <v>54.936613477739066</v>
+        <v>80.917995600193819</v>
       </c>
       <c r="P46" s="2">
         <f t="shared" si="16"/>
-        <v>21.987593162649013</v>
+        <v>1.3027049323209996</v>
       </c>
       <c r="Q46" s="2">
         <f t="shared" si="17"/>
-        <v>112.36589485509268</v>
+        <v>96.985966780014692</v>
       </c>
       <c r="R46" s="2">
         <f t="shared" si="18"/>
-        <v>4.6890930000000015</v>
+        <v>1.1413609999999998</v>
       </c>
       <c r="S46">
         <v>12.385052</v>
@@ -7017,14 +7017,14 @@
         <v>31</v>
       </c>
       <c r="H47">
-        <v>15.468318</v>
+        <v>19.143405999999999</v>
       </c>
       <c r="I47">
         <v>20.471126999999999</v>
       </c>
       <c r="J47" s="2">
         <f t="shared" si="10"/>
-        <v>5.0028089999999992</v>
+        <v>1.3277210000000004</v>
       </c>
       <c r="K47" s="2">
         <f t="shared" si="11"/>
@@ -7032,7 +7032,7 @@
       </c>
       <c r="L47" s="2">
         <f t="shared" si="12"/>
-        <v>6.0501460555555546</v>
+        <v>8.9731013472222187</v>
       </c>
       <c r="M47" s="2">
         <f t="shared" si="13"/>
@@ -7040,23 +7040,23 @@
       </c>
       <c r="N47" s="2">
         <f t="shared" si="14"/>
-        <v>36.604267293554436</v>
+        <v>80.516547787521191</v>
       </c>
       <c r="O47" s="2">
         <f t="shared" si="15"/>
-        <v>58.966833361851513</v>
+        <v>87.454974974496196</v>
       </c>
       <c r="P47" s="2">
         <f t="shared" si="16"/>
-        <v>25.028097890480993</v>
+        <v>1.7628430538410009</v>
       </c>
       <c r="Q47" s="2">
         <f t="shared" si="17"/>
-        <v>122.16781546013108</v>
+        <v>106.10694102903267</v>
       </c>
       <c r="R47" s="2">
         <f t="shared" si="18"/>
-        <v>5.0028089999999992</v>
+        <v>1.3277210000000004</v>
       </c>
       <c r="S47">
         <v>14.474914999999999</v>
@@ -7084,14 +7084,14 @@
         <v>30</v>
       </c>
       <c r="H48">
-        <v>12.845349000000001</v>
+        <v>15.331623</v>
       </c>
       <c r="I48">
         <v>16.325657</v>
       </c>
       <c r="J48" s="2">
         <f t="shared" si="10"/>
-        <v>3.4803079999999991</v>
+        <v>0.9940339999999992</v>
       </c>
       <c r="K48" s="2">
         <f t="shared" si="11"/>
@@ -7099,7 +7099,7 @@
       </c>
       <c r="L48" s="2">
         <f t="shared" si="12"/>
-        <v>3.4271770555555552</v>
+        <v>5.1613183472222204</v>
       </c>
       <c r="M48" s="2">
         <f t="shared" si="13"/>
@@ -7107,23 +7107,23 @@
       </c>
       <c r="N48" s="2">
         <f t="shared" si="14"/>
-        <v>11.745542570126444</v>
+        <v>26.639207081372714</v>
       </c>
       <c r="O48" s="2">
         <f t="shared" si="15"/>
-        <v>19.195203095349004</v>
+        <v>28.907918181257088</v>
       </c>
       <c r="P48" s="2">
         <f t="shared" si="16"/>
-        <v>12.112543774863994</v>
+        <v>0.98810359315599838</v>
       </c>
       <c r="Q48" s="2">
         <f t="shared" si="17"/>
-        <v>47.713349792723321</v>
+        <v>37.888362518454088</v>
       </c>
       <c r="R48" s="2">
         <f t="shared" si="18"/>
-        <v>3.4803079999999991</v>
+        <v>0.9940339999999992</v>
       </c>
       <c r="S48">
         <v>14.355328</v>
@@ -7151,14 +7151,14 @@
         <v>31</v>
       </c>
       <c r="H49">
-        <v>9.2232450000000004</v>
+        <v>9.8799829999999993</v>
       </c>
       <c r="I49">
         <v>8.9291060000000009</v>
       </c>
       <c r="J49" s="2">
         <f t="shared" si="10"/>
-        <v>-0.29413899999999948</v>
+        <v>-0.95087699999999842</v>
       </c>
       <c r="K49" s="2">
         <f t="shared" si="11"/>
@@ -7166,7 +7166,7 @@
       </c>
       <c r="L49" s="2">
         <f t="shared" si="12"/>
-        <v>-0.19492694444444503</v>
+        <v>-0.29032165277778077</v>
       </c>
       <c r="M49" s="2">
         <f t="shared" si="13"/>
@@ -7174,23 +7174,23 @@
       </c>
       <c r="N49" s="2">
         <f t="shared" si="14"/>
-        <v>3.7996513670447755E-2</v>
+        <v>8.4286662071622304E-2</v>
       </c>
       <c r="O49" s="2">
         <f t="shared" si="15"/>
-        <v>0.35002490762349964</v>
+        <v>0.52132253949944052</v>
       </c>
       <c r="P49" s="2">
         <f t="shared" si="16"/>
-        <v>8.6517751320999703E-2</v>
+        <v>0.90416706912899703</v>
       </c>
       <c r="Q49" s="2">
         <f t="shared" si="17"/>
-        <v>0.23918549801533648</v>
+        <v>1.5405740956573741</v>
       </c>
       <c r="R49" s="2">
         <f t="shared" si="18"/>
-        <v>0.29413899999999948</v>
+        <v>0.95087699999999842</v>
       </c>
       <c r="S49">
         <v>10.698161000000001</v>
@@ -7218,14 +7218,14 @@
         <v>30</v>
       </c>
       <c r="H50">
-        <v>6.4217240000000002</v>
+        <v>5.785768</v>
       </c>
       <c r="I50">
         <v>7.0151490000000001</v>
       </c>
       <c r="J50" s="2">
         <f t="shared" si="10"/>
-        <v>0.59342499999999987</v>
+        <v>1.2293810000000001</v>
       </c>
       <c r="K50" s="2">
         <f t="shared" si="11"/>
@@ -7233,7 +7233,7 @@
       </c>
       <c r="L50" s="2">
         <f t="shared" si="12"/>
-        <v>-2.9964479444444452</v>
+        <v>-4.38453665277778</v>
       </c>
       <c r="M50" s="2">
         <f t="shared" si="13"/>
@@ -7241,23 +7241,23 @@
       </c>
       <c r="N50" s="2">
         <f t="shared" si="14"/>
-        <v>8.97870028376534</v>
+        <v>19.224161659551779</v>
       </c>
       <c r="O50" s="2">
         <f t="shared" si="15"/>
-        <v>11.115710982430814</v>
+        <v>16.26500547573788</v>
       </c>
       <c r="P50" s="2">
         <f t="shared" si="16"/>
-        <v>0.35215323062499987</v>
+        <v>1.5113776431610002</v>
       </c>
       <c r="Q50" s="2">
         <f t="shared" si="17"/>
-        <v>5.7745192715264517</v>
+        <v>9.9550071932555788</v>
       </c>
       <c r="R50" s="2">
         <f t="shared" si="18"/>
-        <v>0.59342499999999987</v>
+        <v>1.2293810000000001</v>
       </c>
       <c r="S50">
         <v>5.870679</v>
@@ -7285,14 +7285,14 @@
         <v>31</v>
       </c>
       <c r="H51">
-        <v>4.9075059999999997</v>
+        <v>3.7002160000000002</v>
       </c>
       <c r="I51">
         <v>4.1214890000000004</v>
       </c>
       <c r="J51" s="2">
         <f t="shared" si="10"/>
-        <v>-0.7860169999999993</v>
+        <v>0.42127300000000023</v>
       </c>
       <c r="K51" s="2">
         <f t="shared" si="11"/>
@@ -7300,7 +7300,7 @@
       </c>
       <c r="L51" s="2">
         <f t="shared" si="12"/>
-        <v>-4.5106659444444457</v>
+        <v>-6.4700886527777799</v>
       </c>
       <c r="M51" s="2">
         <f t="shared" si="13"/>
@@ -7308,23 +7308,23 @@
       </c>
       <c r="N51" s="2">
         <f t="shared" si="14"/>
-        <v>20.346107262370904</v>
+        <v>41.862047174803784</v>
       </c>
       <c r="O51" s="2">
         <f t="shared" si="15"/>
-        <v>29.785232003939232</v>
+        <v>42.723866937296819</v>
       </c>
       <c r="P51" s="2">
         <f t="shared" si="16"/>
-        <v>0.61782272428899887</v>
+        <v>0.1774709405290002</v>
       </c>
       <c r="Q51" s="2">
         <f t="shared" si="17"/>
-        <v>28.054850213968674</v>
+        <v>36.588170801289479</v>
       </c>
       <c r="R51" s="2">
         <f t="shared" si="18"/>
-        <v>0.7860169999999993</v>
+        <v>0.42127300000000023</v>
       </c>
       <c r="S51">
         <v>3.4921540000000002</v>
@@ -7352,14 +7352,14 @@
         <v>31</v>
       </c>
       <c r="H52">
-        <v>6.6897539999999998</v>
+        <v>6.1772119999999999</v>
       </c>
       <c r="I52">
         <v>5.2719950000000004</v>
       </c>
       <c r="J52" s="2">
         <f t="shared" si="10"/>
-        <v>-1.4177589999999993</v>
+        <v>-0.90521699999999949</v>
       </c>
       <c r="K52" s="2">
         <f t="shared" si="11"/>
@@ -7367,7 +7367,7 @@
       </c>
       <c r="L52" s="2">
         <f t="shared" si="12"/>
-        <v>-2.7284179444444456</v>
+        <v>-3.9930926527777801</v>
       </c>
       <c r="M52" s="2">
         <f t="shared" si="13"/>
@@ -7375,23 +7375,23 @@
       </c>
       <c r="N52" s="2">
         <f t="shared" si="14"/>
-        <v>7.4442644795664537</v>
+        <v>15.944788933667889</v>
       </c>
       <c r="O52" s="2">
         <f t="shared" si="15"/>
-        <v>14.87747170436079</v>
+        <v>21.773468788224353</v>
       </c>
       <c r="P52" s="2">
         <f t="shared" si="16"/>
-        <v>2.0100405820809981</v>
+        <v>0.81941781708899908</v>
       </c>
       <c r="Q52" s="2">
         <f t="shared" si="17"/>
-        <v>17.190783254642675</v>
+        <v>23.993437454495972</v>
       </c>
       <c r="R52" s="2">
         <f t="shared" si="18"/>
-        <v>1.4177589999999993</v>
+        <v>0.90521699999999949</v>
       </c>
       <c r="S52">
         <v>1.1970860000000001</v>
@@ -7419,14 +7419,14 @@
         <v>28</v>
       </c>
       <c r="H53">
-        <v>5.1091240000000004</v>
+        <v>3.8808240000000001</v>
       </c>
       <c r="I53">
         <v>5.0948130000000003</v>
       </c>
       <c r="J53" s="2">
         <f t="shared" si="10"/>
-        <v>-1.4311000000000185E-2</v>
+        <v>1.2139890000000002</v>
       </c>
       <c r="K53" s="2">
         <f t="shared" si="11"/>
@@ -7434,7 +7434,7 @@
       </c>
       <c r="L53" s="2">
         <f t="shared" si="12"/>
-        <v>-4.3090479444444449</v>
+        <v>-6.2894806527777796</v>
       </c>
       <c r="M53" s="2">
         <f t="shared" si="13"/>
@@ -7442,23 +7442,23 @@
       </c>
       <c r="N53" s="2">
         <f t="shared" si="14"/>
-        <v>18.567894187520896</v>
+        <v>39.557566881666006</v>
       </c>
       <c r="O53" s="2">
         <f t="shared" si="15"/>
-        <v>24.259790247654031</v>
+        <v>35.409557603040099</v>
       </c>
       <c r="P53" s="2">
         <f t="shared" si="16"/>
-        <v>2.0480472100000528E-4</v>
+        <v>1.4737692921210006</v>
       </c>
       <c r="Q53" s="2">
         <f t="shared" si="17"/>
-        <v>18.691432562507785</v>
+        <v>25.76061551741692</v>
       </c>
       <c r="R53" s="2">
         <f t="shared" si="18"/>
-        <v>1.4311000000000185E-2</v>
+        <v>1.2139890000000002</v>
       </c>
       <c r="S53">
         <v>2.6418699999999999</v>
@@ -7486,14 +7486,14 @@
         <v>31</v>
       </c>
       <c r="H54">
-        <v>6.7198719999999996</v>
+        <v>6.1220439999999998</v>
       </c>
       <c r="I54">
         <v>6.727627</v>
       </c>
       <c r="J54" s="2">
         <f t="shared" si="10"/>
-        <v>7.7550000000004005E-3</v>
+        <v>0.6055830000000002</v>
       </c>
       <c r="K54" s="2">
         <f t="shared" si="11"/>
@@ -7501,7 +7501,7 @@
       </c>
       <c r="L54" s="2">
         <f t="shared" si="12"/>
-        <v>-2.6982999444444458</v>
+        <v>-4.0482606527777802</v>
       </c>
       <c r="M54" s="2">
         <f t="shared" si="13"/>
@@ -7509,23 +7509,23 @@
       </c>
       <c r="N54" s="2">
         <f t="shared" si="14"/>
-        <v>7.2808225901888992</v>
+        <v>16.388414312828779</v>
       </c>
       <c r="O54" s="2">
         <f t="shared" si="15"/>
-        <v>10.785513033287428</v>
+        <v>16.181510184802352</v>
       </c>
       <c r="P54" s="2">
         <f t="shared" si="16"/>
-        <v>6.0140025000006212E-5</v>
+        <v>0.36673076988900027</v>
       </c>
       <c r="Q54" s="2">
         <f t="shared" si="17"/>
-        <v>7.2390320980755636</v>
+        <v>11.852029420935525</v>
       </c>
       <c r="R54" s="2">
         <f t="shared" si="18"/>
-        <v>7.7550000000004005E-3</v>
+        <v>0.6055830000000002</v>
       </c>
       <c r="S54">
         <v>4.3188110000000002</v>
@@ -7553,14 +7553,14 @@
         <v>30</v>
       </c>
       <c r="H55">
-        <v>8.1393380000000004</v>
+        <v>8.2367699999999999</v>
       </c>
       <c r="I55">
         <v>8.0741010000000006</v>
       </c>
       <c r="J55" s="2">
         <f t="shared" si="10"/>
-        <v>-6.5236999999999767E-2</v>
+        <v>-0.16266899999999929</v>
       </c>
       <c r="K55" s="2">
         <f t="shared" si="11"/>
@@ -7568,7 +7568,7 @@
       </c>
       <c r="L55" s="2">
         <f t="shared" si="12"/>
-        <v>-1.278833944444445</v>
+        <v>-1.9335346527777801</v>
       </c>
       <c r="M55" s="2">
         <f t="shared" si="13"/>
@@ -7576,23 +7576,23 @@
       </c>
       <c r="N55" s="2">
         <f t="shared" si="14"/>
-        <v>1.6354162574633377</v>
+        <v>3.738556253492491</v>
       </c>
       <c r="O55" s="2">
         <f t="shared" si="15"/>
-        <v>3.389776060828233</v>
+        <v>5.1251763430593531</v>
       </c>
       <c r="P55" s="2">
         <f t="shared" si="16"/>
-        <v>4.2558661689999699E-3</v>
+        <v>2.6461203560999767E-2</v>
       </c>
       <c r="Q55" s="2">
         <f t="shared" si="17"/>
-        <v>1.8065267036997816</v>
+        <v>4.3940697539189051</v>
       </c>
       <c r="R55" s="2">
         <f t="shared" si="18"/>
-        <v>6.5236999999999767E-2</v>
+        <v>0.16266899999999929</v>
       </c>
       <c r="S55">
         <v>5.710909</v>
@@ -7620,14 +7620,14 @@
         <v>31</v>
       </c>
       <c r="H56">
-        <v>10.965527</v>
+        <v>12.453976000000001</v>
       </c>
       <c r="I56">
         <v>10.960146</v>
       </c>
       <c r="J56" s="2">
         <f t="shared" si="10"/>
-        <v>-5.3809999999998581E-3</v>
+        <v>-1.4938300000000009</v>
       </c>
       <c r="K56" s="2">
         <f t="shared" si="11"/>
@@ -7635,7 +7635,7 @@
       </c>
       <c r="L56" s="2">
         <f t="shared" si="12"/>
-        <v>1.5473550555555544</v>
+        <v>2.2836713472222208</v>
       </c>
       <c r="M56" s="2">
         <f t="shared" si="13"/>
@@ -7643,23 +7643,23 @@
       </c>
       <c r="N56" s="2">
         <f t="shared" si="14"/>
-        <v>2.3943076679533331</v>
+        <v>5.2151548221237531</v>
       </c>
       <c r="O56" s="2">
         <f t="shared" si="15"/>
-        <v>0.3641974563861971</v>
+        <v>0.53750255501751076</v>
       </c>
       <c r="P56" s="2">
         <f t="shared" si="16"/>
-        <v>2.8955160999998472E-5</v>
+        <v>2.2315280689000025</v>
       </c>
       <c r="Q56" s="2">
         <f t="shared" si="17"/>
-        <v>2.3776839880064444</v>
+        <v>0.62384935378181128</v>
       </c>
       <c r="R56" s="2">
         <f t="shared" si="18"/>
-        <v>5.3809999999998581E-3</v>
+        <v>1.4938300000000009</v>
       </c>
       <c r="S56">
         <v>7.193924</v>
@@ -7687,14 +7687,14 @@
         <v>30</v>
       </c>
       <c r="H57">
-        <v>12.090954999999999</v>
+        <v>14.089005999999999</v>
       </c>
       <c r="I57">
         <v>14.537305</v>
       </c>
       <c r="J57" s="2">
         <f t="shared" si="10"/>
-        <v>2.4463500000000007</v>
+        <v>0.44829900000000045</v>
       </c>
       <c r="K57" s="2">
         <f t="shared" si="11"/>
@@ -7702,7 +7702,7 @@
       </c>
       <c r="L57" s="2">
         <f t="shared" si="12"/>
-        <v>2.6727830555555538</v>
+        <v>3.9187013472222194</v>
       </c>
       <c r="M57" s="2">
         <f t="shared" si="13"/>
@@ -7710,23 +7710,23 @@
       </c>
       <c r="N57" s="2">
         <f t="shared" si="14"/>
-        <v>7.1437692620648825</v>
+        <v>15.356220248721238</v>
       </c>
       <c r="O57" s="2">
         <f t="shared" si="15"/>
-        <v>10.190056859130305</v>
+        <v>14.940153657119351</v>
       </c>
       <c r="P57" s="2">
         <f t="shared" si="16"/>
-        <v>5.9846283225000034</v>
+        <v>0.20097199340100039</v>
       </c>
       <c r="Q57" s="2">
         <f t="shared" si="17"/>
-        <v>26.205523240481547</v>
+        <v>19.070692032638988</v>
       </c>
       <c r="R57" s="2">
         <f t="shared" si="18"/>
-        <v>2.4463500000000007</v>
+        <v>0.44829900000000045</v>
       </c>
       <c r="S57">
         <v>8.9577299999999997</v>
@@ -7754,14 +7754,14 @@
         <v>31</v>
       </c>
       <c r="H58">
-        <v>15.754887</v>
+        <v>19.526872999999998</v>
       </c>
       <c r="I58">
         <v>18.976659999999999</v>
       </c>
       <c r="J58" s="2">
         <f t="shared" si="10"/>
-        <v>3.2217729999999989</v>
+        <v>-0.5502129999999994</v>
       </c>
       <c r="K58" s="2">
         <f t="shared" si="11"/>
@@ -7769,7 +7769,7 @@
       </c>
       <c r="L58" s="2">
         <f t="shared" si="12"/>
-        <v>6.3367150555555547</v>
+        <v>9.3565683472222183</v>
       </c>
       <c r="M58" s="2">
         <f t="shared" si="13"/>
@@ -7777,23 +7777,23 @@
       </c>
       <c r="N58" s="2">
         <f t="shared" si="14"/>
-        <v>40.153957695304435</v>
+        <v>87.545371236240712</v>
       </c>
       <c r="O58" s="2">
         <f t="shared" si="15"/>
-        <v>52.289823233879197</v>
+        <v>77.209295457118358</v>
       </c>
       <c r="P58" s="2">
         <f t="shared" si="16"/>
-        <v>10.379821263528992</v>
+        <v>0.30273434536899935</v>
       </c>
       <c r="Q58" s="2">
         <f t="shared" si="17"/>
-        <v>91.364693908198191</v>
+        <v>77.55189450154937</v>
       </c>
       <c r="R58" s="2">
         <f t="shared" si="18"/>
-        <v>3.2217729999999989</v>
+        <v>0.5502129999999994</v>
       </c>
       <c r="S58">
         <v>11.752560000000001</v>
@@ -7821,14 +7821,14 @@
         <v>31</v>
       </c>
       <c r="H59">
-        <v>15.936168</v>
+        <v>19.820018999999998</v>
       </c>
       <c r="I59">
         <v>21.242239000000001</v>
       </c>
       <c r="J59" s="2">
         <f t="shared" si="10"/>
-        <v>5.3060710000000011</v>
+        <v>1.4222200000000029</v>
       </c>
       <c r="K59" s="2">
         <f t="shared" si="11"/>
@@ -7836,7 +7836,7 @@
       </c>
       <c r="L59" s="2">
         <f t="shared" si="12"/>
-        <v>6.5179960555555549</v>
+        <v>9.6497143472222184</v>
       </c>
       <c r="M59" s="2">
         <f t="shared" si="13"/>
@@ -7844,23 +7844,23 @@
       </c>
       <c r="N59" s="2">
         <f t="shared" si="14"/>
-        <v>42.484272580237771</v>
+        <v>93.116986982986319</v>
       </c>
       <c r="O59" s="2">
         <f t="shared" si="15"/>
-        <v>68.552767592432673</v>
+        <v>101.49049176159778</v>
       </c>
       <c r="P59" s="2">
         <f t="shared" si="16"/>
-        <v>28.154389457041013</v>
+        <v>2.0227097284000082</v>
       </c>
       <c r="Q59" s="2">
         <f t="shared" si="17"/>
-        <v>139.80856173427424</v>
+        <v>122.58773018919916</v>
       </c>
       <c r="R59" s="2">
         <f t="shared" si="18"/>
-        <v>5.3060710000000011</v>
+        <v>1.4222200000000029</v>
       </c>
       <c r="S59">
         <v>13.397656</v>
@@ -7888,14 +7888,14 @@
         <v>30</v>
       </c>
       <c r="H60">
-        <v>13.682073000000001</v>
+        <v>16.607327000000002</v>
       </c>
       <c r="I60">
         <v>17.225871999999999</v>
       </c>
       <c r="J60" s="2">
         <f t="shared" si="10"/>
-        <v>3.5437989999999981</v>
+        <v>0.61854499999999746</v>
       </c>
       <c r="K60" s="2">
         <f t="shared" si="11"/>
@@ -7903,7 +7903,7 @@
       </c>
       <c r="L60" s="2">
         <f t="shared" si="12"/>
-        <v>4.2639010555555554</v>
+        <v>6.4370223472222214</v>
       </c>
       <c r="M60" s="2">
         <f t="shared" si="13"/>
@@ -7911,23 +7911,23 @@
       </c>
       <c r="N60" s="2">
         <f t="shared" si="14"/>
-        <v>18.180852211567778</v>
+        <v>41.435256698638277</v>
       </c>
       <c r="O60" s="2">
         <f t="shared" si="15"/>
-        <v>27.720020443669782</v>
+        <v>41.847685660733632</v>
       </c>
       <c r="P60" s="2">
         <f t="shared" si="16"/>
-        <v>12.558511352400988</v>
+        <v>0.38259791702499685</v>
       </c>
       <c r="Q60" s="2">
         <f t="shared" si="17"/>
-        <v>60.960180157522196</v>
+        <v>49.781030591188376</v>
       </c>
       <c r="R60" s="2">
         <f t="shared" si="18"/>
-        <v>3.5437989999999981</v>
+        <v>0.61854499999999746</v>
       </c>
       <c r="S60">
         <v>13.115736999999999</v>
@@ -7955,14 +7955,14 @@
         <v>31</v>
       </c>
       <c r="H61">
-        <v>11.03308</v>
+        <v>12.605307</v>
       </c>
       <c r="I61">
         <v>12.562853</v>
       </c>
       <c r="J61" s="2">
         <f t="shared" si="10"/>
-        <v>1.5297730000000005</v>
+        <v>-4.2453999999999326E-2</v>
       </c>
       <c r="K61" s="2">
         <f t="shared" si="11"/>
@@ -7970,7 +7970,7 @@
       </c>
       <c r="L61" s="2">
         <f t="shared" si="12"/>
-        <v>1.6149080555555546</v>
+        <v>2.4350023472222198</v>
       </c>
       <c r="M61" s="2">
         <f t="shared" si="13"/>
@@ -7978,23 +7978,23 @@
       </c>
       <c r="N61" s="2">
         <f t="shared" si="14"/>
-        <v>2.6079280278982222</v>
+        <v>5.9292364309777197</v>
       </c>
       <c r="O61" s="2">
         <f t="shared" si="15"/>
-        <v>2.9683216980589884</v>
+        <v>4.4757162968004245</v>
       </c>
       <c r="P61" s="2">
         <f t="shared" si="16"/>
-        <v>2.3402054315290015</v>
+        <v>1.8023421159999427E-3</v>
       </c>
       <c r="Q61" s="2">
         <f t="shared" si="17"/>
-        <v>9.8890189411700007</v>
+        <v>5.7242875937957782</v>
       </c>
       <c r="R61" s="2">
         <f t="shared" si="18"/>
-        <v>1.5297730000000005</v>
+        <v>4.2453999999999326E-2</v>
       </c>
       <c r="S61">
         <v>9.924175</v>
@@ -8022,14 +8022,14 @@
         <v>30</v>
       </c>
       <c r="H62">
-        <v>6.8393689999999996</v>
+        <v>6.3983939999999997</v>
       </c>
       <c r="I62">
         <v>7.6315049999999998</v>
       </c>
       <c r="J62" s="2">
         <f t="shared" si="10"/>
-        <v>0.79213600000000017</v>
+        <v>1.2331110000000001</v>
       </c>
       <c r="K62" s="2">
         <f t="shared" si="11"/>
@@ -8037,7 +8037,7 @@
       </c>
       <c r="L62" s="2">
         <f t="shared" si="12"/>
-        <v>-2.5788029444444458</v>
+        <v>-3.7719106527777804</v>
       </c>
       <c r="M62" s="2">
         <f t="shared" si="13"/>
@@ -8045,23 +8045,23 @@
       </c>
       <c r="N62" s="2">
         <f t="shared" si="14"/>
-        <v>6.6502246262753433</v>
+        <v>14.227309972538501</v>
       </c>
       <c r="O62" s="2">
         <f t="shared" si="15"/>
-        <v>7.976942200887942</v>
+        <v>11.667550376015186</v>
       </c>
       <c r="P62" s="2">
         <f t="shared" si="16"/>
-        <v>0.62747944249600029</v>
+        <v>1.5205627383210001</v>
       </c>
       <c r="Q62" s="2">
         <f t="shared" si="17"/>
-        <v>3.1921787703704516</v>
+        <v>6.4455036769445782</v>
       </c>
       <c r="R62" s="2">
         <f t="shared" si="18"/>
-        <v>0.79213600000000017</v>
+        <v>1.2331110000000001</v>
       </c>
       <c r="S62">
         <v>4.5283889999999998</v>
@@ -8089,14 +8089,14 @@
         <v>31</v>
       </c>
       <c r="H63">
-        <v>6.1479119999999998</v>
+        <v>5.3554399999999998</v>
       </c>
       <c r="I63">
         <v>7.4172419999999999</v>
       </c>
       <c r="J63" s="2">
         <f t="shared" si="10"/>
-        <v>1.2693300000000001</v>
+        <v>2.0618020000000001</v>
       </c>
       <c r="K63" s="2">
         <f t="shared" si="11"/>
@@ -8104,7 +8104,7 @@
       </c>
       <c r="L63" s="2">
         <f t="shared" si="12"/>
-        <v>-3.2702599444444456</v>
+        <v>-4.8148646527777803</v>
       </c>
       <c r="M63" s="2">
         <f t="shared" si="13"/>
@@ -8112,23 +8112,23 @@
       </c>
       <c r="N63" s="2">
         <f t="shared" si="14"/>
-        <v>10.694600104237788</v>
+        <v>23.182921624568895</v>
       </c>
       <c r="O63" s="2">
         <f t="shared" si="15"/>
-        <v>10.816503358593259</v>
+        <v>15.925339444779281</v>
       </c>
       <c r="P63" s="2">
         <f t="shared" si="16"/>
-        <v>1.6111986489000001</v>
+        <v>4.2510274872040004</v>
       </c>
       <c r="Q63" s="2">
         <f t="shared" si="17"/>
-        <v>4.0037206425744518</v>
+        <v>7.5793539701198283</v>
       </c>
       <c r="R63" s="2">
         <f t="shared" si="18"/>
-        <v>1.2693300000000001</v>
+        <v>2.0618020000000001</v>
       </c>
       <c r="S63">
         <v>2.3634759999999999</v>
@@ -8156,14 +8156,14 @@
         <v>31</v>
       </c>
       <c r="H64">
-        <v>7.7735810000000001</v>
+        <v>7.7686400000000004</v>
       </c>
       <c r="I64">
         <v>6.6338660000000003</v>
       </c>
       <c r="J64" s="2">
         <f t="shared" si="10"/>
-        <v>-1.1397149999999998</v>
+        <v>-1.1347740000000002</v>
       </c>
       <c r="K64" s="2">
         <f t="shared" si="11"/>
@@ -8171,7 +8171,7 @@
       </c>
       <c r="L64" s="2">
         <f t="shared" si="12"/>
-        <v>-1.6445909444444453</v>
+        <v>-2.4016646527777796</v>
       </c>
       <c r="M64" s="2">
         <f t="shared" si="13"/>
@@ -8179,23 +8179,23 @@
       </c>
       <c r="N64" s="2">
         <f t="shared" si="14"/>
-        <v>2.7046793745486726</v>
+        <v>5.7679931044022128</v>
       </c>
       <c r="O64" s="2">
         <f t="shared" si="15"/>
-        <v>6.727877263708387</v>
+        <v>9.8249993817970616</v>
       </c>
       <c r="P64" s="2">
         <f t="shared" si="16"/>
-        <v>1.2989502812249996</v>
+        <v>1.2877120310760004</v>
       </c>
       <c r="Q64" s="2">
         <f t="shared" si="17"/>
-        <v>7.7523595922686734</v>
+        <v>12.506398344860719</v>
       </c>
       <c r="R64" s="2">
         <f t="shared" si="18"/>
-        <v>1.1397149999999998</v>
+        <v>1.1347740000000002</v>
       </c>
       <c r="S64">
         <v>4.4663490000000001</v>
@@ -8223,14 +8223,14 @@
         <v>28</v>
       </c>
       <c r="H65">
-        <v>7.9811069999999997</v>
+        <v>8.0858450000000008</v>
       </c>
       <c r="I65">
         <v>7.2626730000000004</v>
       </c>
       <c r="J65" s="2">
         <f t="shared" si="10"/>
-        <v>-0.71843399999999935</v>
+        <v>-0.82317200000000046</v>
       </c>
       <c r="K65" s="2">
         <f t="shared" si="11"/>
@@ -8238,7 +8238,7 @@
       </c>
       <c r="L65" s="2">
         <f t="shared" si="12"/>
-        <v>-1.4370649444444457</v>
+        <v>-2.0844596527777792</v>
       </c>
       <c r="M65" s="2">
         <f t="shared" si="13"/>
@@ -8246,23 +8246,23 @@
       </c>
       <c r="N65" s="2">
         <f t="shared" si="14"/>
-        <v>2.0651556545511176</v>
+        <v>4.3449720440584603</v>
       </c>
       <c r="O65" s="2">
         <f t="shared" si="15"/>
-        <v>4.9752701087113049</v>
+        <v>7.2166187362459491</v>
       </c>
       <c r="P65" s="2">
         <f t="shared" si="16"/>
-        <v>0.51614741235599904</v>
+        <v>0.67761214158400074</v>
       </c>
       <c r="Q65" s="2">
         <f t="shared" si="17"/>
-        <v>4.646175699501117</v>
+        <v>8.4543218282352424</v>
       </c>
       <c r="R65" s="2">
         <f t="shared" si="18"/>
-        <v>0.71843399999999935</v>
+        <v>0.82317200000000046</v>
       </c>
       <c r="S65">
         <v>4.6956059999999997</v>
@@ -8290,14 +8290,14 @@
         <v>31</v>
       </c>
       <c r="H66">
-        <v>8.9005240000000008</v>
+        <v>9.4184230000000007</v>
       </c>
       <c r="I66">
         <v>7.8642589999999997</v>
       </c>
       <c r="J66" s="2">
         <f t="shared" si="10"/>
-        <v>-1.0362650000000011</v>
+        <v>-1.554164000000001</v>
       </c>
       <c r="K66" s="2">
         <f t="shared" si="11"/>
@@ -8305,7 +8305,7 @@
       </c>
       <c r="L66" s="2">
         <f t="shared" si="12"/>
-        <v>-0.51764794444444462</v>
+        <v>-0.75188165277777941</v>
       </c>
       <c r="M66" s="2">
         <f t="shared" si="13"/>
@@ -8313,23 +8313,23 @@
       </c>
       <c r="N66" s="2">
         <f t="shared" si="14"/>
-        <v>0.26795939438755884</v>
+        <v>0.56532601978384522</v>
       </c>
       <c r="O66" s="2">
         <f t="shared" si="15"/>
-        <v>1.480741916995818</v>
+        <v>2.1507719519354529</v>
       </c>
       <c r="P66" s="2">
         <f t="shared" si="16"/>
-        <v>1.0738451502250024</v>
+        <v>2.415425738896003</v>
       </c>
       <c r="Q66" s="2">
         <f t="shared" si="17"/>
-        <v>2.4146454389120069</v>
+        <v>5.3178465526952996</v>
       </c>
       <c r="R66" s="2">
         <f t="shared" si="18"/>
-        <v>1.0362650000000011</v>
+        <v>1.554164000000001</v>
       </c>
       <c r="S66">
         <v>5.3733880000000003</v>
@@ -8357,14 +8357,14 @@
         <v>30</v>
       </c>
       <c r="H67">
-        <v>8.0581899999999997</v>
+        <v>8.124053</v>
       </c>
       <c r="I67">
         <v>8.61557</v>
       </c>
       <c r="J67" s="2">
         <f t="shared" si="10"/>
-        <v>0.55738000000000021</v>
+        <v>0.49151699999999998</v>
       </c>
       <c r="K67" s="2">
         <f t="shared" si="11"/>
@@ -8372,7 +8372,7 @@
       </c>
       <c r="L67" s="2">
         <f t="shared" si="12"/>
-        <v>-1.3599819444444456</v>
+        <v>-2.0462516527777801</v>
       </c>
       <c r="M67" s="2">
         <f t="shared" si="13"/>
@@ -8380,23 +8380,23 @@
       </c>
       <c r="N67" s="2">
         <f t="shared" si="14"/>
-        <v>1.8495508892148953</v>
+        <v>4.1871458264957964</v>
       </c>
       <c r="O67" s="2">
         <f t="shared" si="15"/>
-        <v>2.8684851559619013</v>
+        <v>4.3159708960351857</v>
       </c>
       <c r="P67" s="2">
         <f t="shared" si="16"/>
-        <v>0.31067246440000024</v>
+        <v>0.24158896128899998</v>
       </c>
       <c r="Q67" s="2">
         <f t="shared" si="17"/>
-        <v>0.64416988122600471</v>
+        <v>2.4171998405480446</v>
       </c>
       <c r="R67" s="2">
         <f t="shared" si="18"/>
-        <v>0.55738000000000021</v>
+        <v>0.49151699999999998</v>
       </c>
       <c r="S67">
         <v>6.4953919999999998</v>
@@ -8424,14 +8424,14 @@
         <v>31</v>
       </c>
       <c r="H68">
-        <v>11.277295000000001</v>
+        <v>12.881795</v>
       </c>
       <c r="I68">
         <v>13.252872999999999</v>
       </c>
       <c r="J68" s="2">
         <f t="shared" si="10"/>
-        <v>1.9755779999999987</v>
+        <v>0.37107799999999891</v>
       </c>
       <c r="K68" s="2">
         <f t="shared" si="11"/>
@@ -8439,7 +8439,7 @@
       </c>
       <c r="L68" s="2">
         <f t="shared" si="12"/>
-        <v>1.8591230555555551</v>
+        <v>2.7114903472222203</v>
       </c>
       <c r="M68" s="2">
         <f t="shared" si="13"/>
@@ -8447,23 +8447,23 @@
       </c>
       <c r="N68" s="2">
         <f t="shared" si="14"/>
-        <v>3.4563385356982237</v>
+        <v>7.3521799030792767</v>
       </c>
       <c r="O68" s="2">
         <f t="shared" si="15"/>
-        <v>4.7000392105328066</v>
+        <v>6.8549044738285883</v>
       </c>
       <c r="P68" s="2">
         <f t="shared" si="16"/>
-        <v>3.902908434083995</v>
+        <v>0.13769888208399919</v>
       </c>
       <c r="Q68" s="2">
         <f t="shared" si="17"/>
-        <v>14.70493218547888</v>
+        <v>9.5022276152963236</v>
       </c>
       <c r="R68" s="2">
         <f t="shared" si="18"/>
-        <v>1.9755779999999987</v>
+        <v>0.37107799999999891</v>
       </c>
       <c r="S68">
         <v>9.6104040000000008</v>
@@ -8491,14 +8491,14 @@
         <v>30</v>
       </c>
       <c r="H69">
-        <v>15.160458</v>
+        <v>18.613572999999999</v>
       </c>
       <c r="I69">
         <v>19.900960999999999</v>
       </c>
       <c r="J69" s="2">
         <f t="shared" si="10"/>
-        <v>4.7405029999999986</v>
+        <v>1.287388</v>
       </c>
       <c r="K69" s="2">
         <f t="shared" si="11"/>
@@ -8506,7 +8506,7 @@
       </c>
       <c r="L69" s="2">
         <f t="shared" si="12"/>
-        <v>5.7422860555555548</v>
+        <v>8.4432683472222188</v>
       </c>
       <c r="M69" s="2">
         <f t="shared" si="13"/>
@@ -8514,23 +8514,23 @@
       </c>
       <c r="N69" s="2">
         <f t="shared" si="14"/>
-        <v>32.973849143827771</v>
+        <v>71.288780383204625</v>
       </c>
       <c r="O69" s="2">
         <f t="shared" si="15"/>
-        <v>52.692266168800458</v>
+        <v>77.47697324413393</v>
       </c>
       <c r="P69" s="2">
         <f t="shared" si="16"/>
-        <v>22.472368693008985</v>
+        <v>1.657367862544</v>
       </c>
       <c r="Q69" s="2">
         <f t="shared" si="17"/>
-        <v>109.88886638327529</v>
+        <v>94.685672947736052</v>
       </c>
       <c r="R69" s="2">
         <f t="shared" si="18"/>
-        <v>4.7405029999999986</v>
+        <v>1.287388</v>
       </c>
       <c r="S69">
         <v>10.771552</v>
@@ -8558,14 +8558,14 @@
         <v>31</v>
       </c>
       <c r="H70">
-        <v>16.247042</v>
+        <v>20.134067999999999</v>
       </c>
       <c r="I70">
         <v>22.769897</v>
       </c>
       <c r="J70" s="2">
         <f t="shared" si="10"/>
-        <v>6.5228549999999998</v>
+        <v>2.6358290000000011</v>
       </c>
       <c r="K70" s="2">
         <f t="shared" si="11"/>
@@ -8573,7 +8573,7 @@
       </c>
       <c r="L70" s="2">
         <f t="shared" si="12"/>
-        <v>6.828870055555555</v>
+        <v>9.9637633472222191</v>
       </c>
       <c r="M70" s="2">
         <f t="shared" si="13"/>
@@ -8581,23 +8581,23 @@
       </c>
       <c r="N70" s="2">
         <f t="shared" si="14"/>
-        <v>46.633466235663327</v>
+        <v>99.276580039448916</v>
       </c>
       <c r="O70" s="2">
         <f t="shared" si="15"/>
-        <v>82.254550652640361</v>
+        <v>120.01471257580354</v>
       </c>
       <c r="P70" s="2">
         <f t="shared" si="16"/>
-        <v>42.547637351024996</v>
+        <v>6.9475945172410061</v>
       </c>
       <c r="Q70" s="2">
         <f t="shared" si="17"/>
-        <v>178.26856195914999</v>
+        <v>158.74972731618072</v>
       </c>
       <c r="R70" s="2">
         <f t="shared" si="18"/>
-        <v>6.5228549999999998</v>
+        <v>2.6358290000000011</v>
       </c>
       <c r="S70">
         <v>13.215975</v>
@@ -8625,14 +8625,14 @@
         <v>31</v>
       </c>
       <c r="H71">
-        <v>15.759136</v>
+        <v>19.531728999999999</v>
       </c>
       <c r="I71">
         <v>21.078575000000001</v>
       </c>
       <c r="J71" s="2">
         <f t="shared" si="10"/>
-        <v>5.3194390000000009</v>
+        <v>1.5468460000000022</v>
       </c>
       <c r="K71" s="2">
         <f t="shared" si="11"/>
@@ -8640,7 +8640,7 @@
       </c>
       <c r="L71" s="2">
         <f t="shared" si="12"/>
-        <v>6.3409640555555544</v>
+        <v>9.3614243472222185</v>
       </c>
       <c r="M71" s="2">
         <f t="shared" si="13"/>
@@ -8648,23 +8648,23 @@
       </c>
       <c r="N71" s="2">
         <f t="shared" si="14"/>
-        <v>40.207825153847544</v>
+        <v>87.636265808764946</v>
       </c>
       <c r="O71" s="2">
         <f t="shared" si="15"/>
-        <v>65.653052942208987</v>
+        <v>96.926284851620522</v>
       </c>
       <c r="P71" s="2">
         <f t="shared" si="16"/>
-        <v>28.296431274721009</v>
+        <v>2.3927325477160069</v>
       </c>
       <c r="Q71" s="2">
         <f t="shared" si="17"/>
-        <v>135.96499941800934</v>
+        <v>118.99036196808758</v>
       </c>
       <c r="R71" s="2">
         <f t="shared" si="18"/>
-        <v>5.3194390000000009</v>
+        <v>1.5468460000000022</v>
       </c>
       <c r="S71">
         <v>15.243527</v>
@@ -8692,14 +8692,14 @@
         <v>30</v>
       </c>
       <c r="H72">
-        <v>12.396628</v>
+        <v>14.65448</v>
       </c>
       <c r="I72">
         <v>16.182568</v>
       </c>
       <c r="J72" s="2">
         <f t="shared" si="10"/>
-        <v>3.7859400000000001</v>
+        <v>1.5280880000000003</v>
       </c>
       <c r="K72" s="2">
         <f t="shared" si="11"/>
@@ -8707,7 +8707,7 @@
       </c>
       <c r="L72" s="2">
         <f t="shared" si="12"/>
-        <v>2.9784560555555544</v>
+        <v>4.4841753472222194</v>
       </c>
       <c r="M72" s="2">
         <f t="shared" si="13"/>
@@ -8715,23 +8715,23 @@
       </c>
       <c r="N72" s="2">
         <f t="shared" si="14"/>
-        <v>8.8712004748755522</v>
+        <v>20.107828544635513</v>
       </c>
       <c r="O72" s="2">
         <f t="shared" si="15"/>
-        <v>16.255786889469096</v>
+        <v>24.473686184991916</v>
       </c>
       <c r="P72" s="2">
         <f t="shared" si="16"/>
-        <v>14.3333416836</v>
+        <v>2.3350529357440011</v>
       </c>
       <c r="Q72" s="2">
         <f t="shared" si="17"/>
-        <v>45.757053996415543</v>
+        <v>36.147310556351727</v>
       </c>
       <c r="R72" s="2">
         <f t="shared" si="18"/>
-        <v>3.7859400000000001</v>
+        <v>1.5280880000000003</v>
       </c>
       <c r="S72">
         <v>14.913529</v>
@@ -8759,14 +8759,14 @@
         <v>31</v>
       </c>
       <c r="H73">
-        <v>11.708904</v>
+        <v>13.600369000000001</v>
       </c>
       <c r="I73">
         <v>13.124743</v>
       </c>
       <c r="J73" s="2">
         <f t="shared" si="10"/>
-        <v>1.4158390000000001</v>
+        <v>-0.4756260000000001</v>
       </c>
       <c r="K73" s="2">
         <f t="shared" si="11"/>
@@ -8774,7 +8774,7 @@
       </c>
       <c r="L73" s="2">
         <f t="shared" si="12"/>
-        <v>2.290732055555555</v>
+        <v>3.4300643472222205</v>
       </c>
       <c r="M73" s="2">
         <f t="shared" si="13"/>
@@ -8782,23 +8782,23 @@
       </c>
       <c r="N73" s="2">
         <f t="shared" si="14"/>
-        <v>5.2474533503497787</v>
+        <v>11.765341426084998</v>
       </c>
       <c r="O73" s="2">
         <f t="shared" si="15"/>
-        <v>5.4976761532126579</v>
+        <v>8.2320334759253164</v>
       </c>
       <c r="P73" s="2">
         <f t="shared" si="16"/>
-        <v>2.0046000739210004</v>
+        <v>0.22622009187600009</v>
       </c>
       <c r="Q73" s="2">
         <f t="shared" si="17"/>
-        <v>13.738668989882221</v>
+        <v>8.7287059475371649</v>
       </c>
       <c r="R73" s="2">
         <f t="shared" si="18"/>
-        <v>1.4158390000000001</v>
+        <v>0.4756260000000001</v>
       </c>
       <c r="S73">
         <v>13.524543</v>
@@ -8826,14 +8826,14 @@
         <v>30</v>
       </c>
       <c r="H74">
-        <v>5.8872299999999997</v>
+        <v>4.9770370000000002</v>
       </c>
       <c r="I74">
         <v>7.4532730000000003</v>
       </c>
       <c r="J74" s="2">
         <f t="shared" si="10"/>
-        <v>1.5660430000000005</v>
+        <v>2.4762360000000001</v>
       </c>
       <c r="K74" s="2">
         <f t="shared" si="11"/>
@@ -8841,7 +8841,7 @@
       </c>
       <c r="L74" s="2">
         <f t="shared" si="12"/>
-        <v>-3.5309419444444456</v>
+        <v>-5.1932676527777799</v>
       </c>
       <c r="M74" s="2">
         <f t="shared" si="13"/>
@@ -8849,23 +8849,23 @@
       </c>
       <c r="N74" s="2">
         <f t="shared" si="14"/>
-        <v>12.467551015037122</v>
+        <v>26.970028913388031</v>
       </c>
       <c r="O74" s="2">
         <f t="shared" si="15"/>
-        <v>11.551495157736063</v>
+        <v>16.989802462846388</v>
       </c>
       <c r="P74" s="2">
         <f t="shared" si="16"/>
-        <v>2.4524906778490014</v>
+        <v>6.1317447276960007</v>
       </c>
       <c r="Q74" s="2">
         <f t="shared" si="17"/>
-        <v>3.8608278618788945</v>
+        <v>7.3822610021963539</v>
       </c>
       <c r="R74" s="2">
         <f t="shared" si="18"/>
-        <v>1.5660430000000005</v>
+        <v>2.4762360000000001</v>
       </c>
       <c r="S74">
         <v>7.9147090000000002</v>
@@ -8893,14 +8893,14 @@
         <v>31</v>
       </c>
       <c r="H75">
-        <v>5.1732170000000002</v>
+        <v>3.8891260000000001</v>
       </c>
       <c r="I75">
         <v>7.6571740000000004</v>
       </c>
       <c r="J75" s="2">
         <f t="shared" si="10"/>
-        <v>2.4839570000000002</v>
+        <v>3.7680480000000003</v>
       </c>
       <c r="K75" s="2">
         <f t="shared" si="11"/>
@@ -8908,7 +8908,7 @@
       </c>
       <c r="L75" s="2">
         <f t="shared" si="12"/>
-        <v>-4.2449549444444452</v>
+        <v>-6.28117865277778</v>
       </c>
       <c r="M75" s="2">
         <f t="shared" si="13"/>
@@ -8916,23 +8916,23 @@
       </c>
       <c r="N75" s="2">
         <f t="shared" si="14"/>
-        <v>18.019642480363341</v>
+        <v>39.45320526811129</v>
       </c>
       <c r="O75" s="2">
         <f t="shared" si="15"/>
-        <v>13.02184188759399</v>
+        <v>19.268170417508966</v>
       </c>
       <c r="P75" s="2">
         <f t="shared" si="16"/>
-        <v>6.1700423778490006</v>
+        <v>14.198185730304003</v>
       </c>
       <c r="Q75" s="2">
         <f t="shared" si="17"/>
-        <v>3.1011137603375607</v>
+        <v>6.3158256779312687</v>
       </c>
       <c r="R75" s="2">
         <f t="shared" si="18"/>
-        <v>2.4839570000000002</v>
+        <v>3.7680480000000003</v>
       </c>
       <c r="S75">
         <v>4.2786520000000001</v>
@@ -8948,7 +8948,7 @@
     </row>
     <row r="76" spans="4:22" x14ac:dyDescent="0.3">
       <c r="H76">
-        <v>5.0393340000000002</v>
+        <v>3.7530060000000001</v>
       </c>
       <c r="I76">
         <v>7.8185159999999998</v>
@@ -8960,7 +8960,7 @@
     </row>
     <row r="77" spans="4:22" x14ac:dyDescent="0.3">
       <c r="H77">
-        <v>6.847105</v>
+        <v>6.3609549999999997</v>
       </c>
       <c r="I77">
         <v>7.8185159999999998</v>
@@ -8972,7 +8972,7 @@
     </row>
     <row r="78" spans="4:22" x14ac:dyDescent="0.3">
       <c r="H78">
-        <v>6.4430290000000001</v>
+        <v>5.7115340000000003</v>
       </c>
       <c r="I78">
         <v>7.8185159999999998</v>
@@ -8984,7 +8984,7 @@
     </row>
     <row r="79" spans="4:22" x14ac:dyDescent="0.3">
       <c r="H79">
-        <v>9.8976039999999994</v>
+        <v>10.877504</v>
       </c>
       <c r="I79">
         <v>7.8185159999999998</v>
@@ -8996,7 +8996,7 @@
     </row>
     <row r="80" spans="4:22" x14ac:dyDescent="0.3">
       <c r="H80">
-        <v>11.171557</v>
+        <v>12.746848</v>
       </c>
       <c r="I80">
         <v>7.8185159999999998</v>
@@ -9008,7 +9008,7 @@
     </row>
     <row r="81" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H81">
-        <v>12.755964000000001</v>
+        <v>15.079478999999999</v>
       </c>
       <c r="I81">
         <v>7.8185159999999998</v>
@@ -9020,7 +9020,7 @@
     </row>
     <row r="82" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H82">
-        <v>13.705755</v>
+        <v>16.463688000000001</v>
       </c>
       <c r="I82">
         <v>7.8185159999999998</v>
@@ -9032,7 +9032,7 @@
     </row>
     <row r="83" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H83">
-        <v>14.816071000000001</v>
+        <v>18.133773999999999</v>
       </c>
       <c r="I83">
         <v>7.8185159999999998</v>
@@ -9044,7 +9044,7 @@
     </row>
     <row r="84" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H84">
-        <v>11.625911</v>
+        <v>13.475885999999999</v>
       </c>
       <c r="I84">
         <v>7.8185159999999998</v>
@@ -9056,7 +9056,7 @@
     </row>
     <row r="85" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H85">
-        <v>8.5778210000000001</v>
+        <v>8.9190860000000001</v>
       </c>
       <c r="I85">
         <v>7.8185159999999998</v>
@@ -9068,7 +9068,7 @@
     </row>
     <row r="86" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H86">
-        <v>7.7236789999999997</v>
+        <v>7.6639989999999996</v>
       </c>
       <c r="I86">
         <v>7.8185159999999998</v>
@@ -9080,7 +9080,7 @@
     </row>
     <row r="87" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H87">
-        <v>3.6380539999999999</v>
+        <v>1.808792</v>
       </c>
       <c r="I87">
         <v>7.8185159999999998</v>
@@ -9092,7 +9092,7 @@
     </row>
     <row r="88" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H88">
-        <v>4.2222350000000004</v>
+        <v>2.705409</v>
       </c>
       <c r="I88">
         <v>7.8185159999999998</v>
@@ -9104,7 +9104,7 @@
     </row>
     <row r="89" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H89">
-        <v>5.236186</v>
+        <v>4.0119020000000001</v>
       </c>
       <c r="I89">
         <v>7.8185159999999998</v>
@@ -9116,7 +9116,7 @@
     </row>
     <row r="90" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H90">
-        <v>6.203246</v>
+        <v>5.369224</v>
       </c>
       <c r="I90">
         <v>7.8185159999999998</v>
@@ -9128,7 +9128,7 @@
     </row>
     <row r="91" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H91">
-        <v>6.7492289999999997</v>
+        <v>6.1563179999999997</v>
       </c>
       <c r="I91">
         <v>7.8185159999999998</v>
@@ -9140,7 +9140,7 @@
     </row>
     <row r="92" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H92">
-        <v>10.600250000000001</v>
+        <v>11.897114</v>
       </c>
       <c r="I92">
         <v>7.8185159999999998</v>
@@ -9152,7 +9152,7 @@
     </row>
     <row r="93" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H93">
-        <v>12.788347</v>
+        <v>15.144710999999999</v>
       </c>
       <c r="I93">
         <v>7.8185159999999998</v>
@@ -9164,7 +9164,7 @@
     </row>
     <row r="94" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H94">
-        <v>15.117838000000001</v>
+        <v>18.398571</v>
       </c>
       <c r="I94">
         <v>7.8185159999999998</v>
@@ -9176,7 +9176,7 @@
     </row>
     <row r="95" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H95">
-        <v>16.258192000000001</v>
+        <v>20.152441</v>
       </c>
       <c r="I95">
         <v>7.8185159999999998</v>
@@ -9188,7 +9188,7 @@
     </row>
     <row r="96" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H96">
-        <v>13.280865</v>
+        <v>15.909276999999999</v>
       </c>
       <c r="I96">
         <v>7.8185159999999998</v>
@@ -9200,7 +9200,7 @@
     </row>
     <row r="97" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H97">
-        <v>9.0894279999999998</v>
+        <v>9.7026559999999993</v>
       </c>
       <c r="I97">
         <v>7.8185159999999998</v>
@@ -9212,7 +9212,7 @@
     </row>
     <row r="98" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H98">
-        <v>6.2278419999999999</v>
+        <v>5.4410220000000002</v>
       </c>
       <c r="I98">
         <v>7.8185159999999998</v>
@@ -9224,7 +9224,7 @@
     </row>
     <row r="99" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H99">
-        <v>5.2048699999999997</v>
+        <v>4.0441940000000001</v>
       </c>
       <c r="I99">
         <v>7.8185159999999998</v>
@@ -9236,7 +9236,7 @@
     </row>
     <row r="100" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H100">
-        <v>6.0451480000000002</v>
+        <v>5.1618069999999996</v>
       </c>
       <c r="I100">
         <v>7.8185159999999998</v>
@@ -9248,7 +9248,7 @@
     </row>
     <row r="101" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H101">
-        <v>5.1232579999999999</v>
+        <v>3.9569990000000002</v>
       </c>
       <c r="I101">
         <v>7.8185159999999998</v>
@@ -9260,7 +9260,7 @@
     </row>
     <row r="102" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H102">
-        <v>5.8095460000000001</v>
+        <v>4.7896400000000003</v>
       </c>
       <c r="I102">
         <v>7.8185159999999998</v>
@@ -9272,7 +9272,7 @@
     </row>
     <row r="103" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H103">
-        <v>7.7612680000000003</v>
+        <v>7.6771289999999999</v>
       </c>
       <c r="I103">
         <v>7.8185159999999998</v>
@@ -9284,7 +9284,7 @@
     </row>
     <row r="104" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H104">
-        <v>11.697730999999999</v>
+        <v>13.463158</v>
       </c>
       <c r="I104">
         <v>7.8185159999999998</v>
@@ -9296,7 +9296,7 @@
     </row>
     <row r="105" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H105">
-        <v>12.691274999999999</v>
+        <v>14.901141000000001</v>
       </c>
       <c r="I105">
         <v>7.8185159999999998</v>
@@ -9308,7 +9308,7 @@
     </row>
     <row r="106" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H106">
-        <v>15.931388</v>
+        <v>19.623201000000002</v>
       </c>
       <c r="I106">
         <v>7.8185159999999998</v>
@@ -9320,7 +9320,7 @@
     </row>
     <row r="107" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H107">
-        <v>15.439244</v>
+        <v>18.838439999999999</v>
       </c>
       <c r="I107">
         <v>7.8185159999999998</v>
@@ -9332,7 +9332,7 @@
     </row>
     <row r="108" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H108">
-        <v>11.955560999999999</v>
+        <v>13.972019</v>
       </c>
       <c r="I108">
         <v>7.8185159999999998</v>
@@ -9344,7 +9344,7 @@
     </row>
     <row r="109" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H109">
-        <v>10.096086</v>
+        <v>11.201335</v>
       </c>
       <c r="I109">
         <v>7.8185159999999998</v>
@@ -9356,7 +9356,7 @@
     </row>
     <row r="110" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H110">
-        <v>7.0206220000000004</v>
+        <v>6.6556240000000004</v>
       </c>
       <c r="I110">
         <v>7.8185159999999998</v>
@@ -9368,7 +9368,7 @@
     </row>
     <row r="111" spans="8:22" x14ac:dyDescent="0.3">
       <c r="H111">
-        <v>4.8143669999999998</v>
+        <v>3.397316</v>
       </c>
       <c r="I111">
         <v>7.8185159999999998</v>

</xml_diff>